<commit_message>
Co-authored-by: Rowin Veneman <r.veneman@student.utwente.nl>
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37804556674-2</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -495,11 +495,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CLDU 970533 9</t>
+          <t>TCLU 481269 6</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>7433</v>
+        <v>4400</v>
       </c>
       <c r="H2" t="n">
         <v>40</v>
@@ -512,7 +512,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37804556674-2</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -526,7 +526,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PCVU 260008 2</t>
+          <t>MEBU 126421 4</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -543,11 +543,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>94000</v>
+        <v>108000</v>
       </c>
       <c r="D4" t="n">
         <v>90</v>
@@ -557,11 +557,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SANU 752914 5</t>
+          <t>HMCU 904434 0</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>19400</v>
+        <v>23200</v>
       </c>
       <c r="H4" t="n">
         <v>40</v>
@@ -574,11 +574,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>94000</v>
+        <v>108000</v>
       </c>
       <c r="D5" t="n">
         <v>90</v>
@@ -588,11 +588,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>OOLU 985274 6</t>
+          <t>CLDU 962913 6</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>19268</v>
+        <v>28836</v>
       </c>
       <c r="H5" t="n">
         <v>40</v>
@@ -605,11 +605,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>37804557351-6</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>60000</v>
+        <v>72000</v>
       </c>
       <c r="D6" t="n">
         <v>60</v>
@@ -619,11 +619,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>EURU 405291 2</t>
+          <t>TKRU 331851 4</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2800</v>
+        <v>2300</v>
       </c>
       <c r="H6" t="n">
         <v>20</v>
@@ -636,11 +636,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>37804557351-6</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>60000</v>
+        <v>72000</v>
       </c>
       <c r="D7" t="n">
         <v>60</v>
@@ -650,11 +650,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>SAIU 641317 0</t>
+          <t>ABEU 260711 5</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>28800</v>
+        <v>25140</v>
       </c>
       <c r="H7" t="n">
         <v>20</v>
@@ -667,11 +667,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>37804557351-6</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>60000</v>
+        <v>72000</v>
       </c>
       <c r="D8" t="n">
         <v>60</v>
@@ -681,11 +681,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TCKU 335523 7</t>
+          <t>GCAU 795043 0</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>28360</v>
+        <v>28120</v>
       </c>
       <c r="H8" t="n">
         <v>20</v>
@@ -698,25 +698,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>33884961566-5</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D9" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>MEBU 330039 4</t>
+          <t>GMCU 238079 0</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>8600</v>
+        <v>4800</v>
       </c>
       <c r="H9" t="n">
         <v>20</v>
@@ -729,28 +729,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33884961566-5</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>BIDU 496338 0</t>
+          <t>LYSU 545712 9</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>32000</v>
+        <v>28386</v>
       </c>
       <c r="H10" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I10" t="inlineStr"/>
     </row>
@@ -760,11 +760,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33884961566-5</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D11" t="n">
         <v>90</v>
@@ -774,14 +774,14 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PCVU 350056 0</t>
+          <t>CLDU 961735 1</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>32800</v>
+        <v>8518</v>
       </c>
       <c r="H11" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
@@ -791,11 +791,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33884961566-5</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D12" t="n">
         <v>90</v>
@@ -805,11 +805,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>EXFU 877422 0</t>
+          <t>NWBU 010529 9</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>32800</v>
+        <v>28020</v>
       </c>
       <c r="H12" t="n">
         <v>20</v>
@@ -822,28 +822,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>37804556642-9</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D13" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E13" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>EISU 942625 5</t>
+          <t>TANU 351116 0</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>18288</v>
+        <v>31750</v>
       </c>
       <c r="H13" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>37804556642-9</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -863,15 +863,15 @@
         <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>FOTU 122285 9</t>
+          <t>TKRU 321509 6</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>32000</v>
+        <v>2300</v>
       </c>
       <c r="H14" t="n">
         <v>20</v>
@@ -884,28 +884,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>31804557061-7</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D15" t="n">
         <v>60</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>SANU 740000 8</t>
+          <t>ABEU 252405 2</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>23540</v>
+        <v>27960</v>
       </c>
       <c r="H15" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I15" t="inlineStr"/>
     </row>
@@ -915,25 +915,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>31804557061-7</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D16" t="n">
         <v>60</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TTNU 142566 7</t>
+          <t>TCLU 226328 3</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>28360</v>
+        <v>28160</v>
       </c>
       <c r="H16" t="n">
         <v>20</v>
@@ -946,7 +946,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33684556902-7</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -956,18 +956,18 @@
         <v>60</v>
       </c>
       <c r="E17" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>TKRU 321319 6</t>
+          <t>LYSU 546249 1</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>2300</v>
+        <v>28386</v>
       </c>
       <c r="H17" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I17" t="inlineStr"/>
     </row>
@@ -977,7 +977,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33684556902-7</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -987,15 +987,15 @@
         <v>60</v>
       </c>
       <c r="E18" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>TWSU 271860 2</t>
+          <t>ILBU 261007 6</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>28960</v>
+        <v>28000</v>
       </c>
       <c r="H18" t="n">
         <v>20</v>
@@ -1008,11 +1008,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33684556902-7</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D19" t="n">
         <v>60</v>
@@ -1022,14 +1022,14 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>ABEU 260183 7</t>
+          <t>CMAU 825245 1</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>34000</v>
+        <v>17011</v>
       </c>
       <c r="H19" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1039,25 +1039,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D20" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MEDU 565772 6</t>
+          <t>COUU 810204 9</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>20248</v>
+        <v>32800</v>
       </c>
       <c r="H20" t="n">
         <v>20</v>
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D21" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E21" t="n">
         <v>12</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>FOTU 643203 5</t>
+          <t>TKRU 317044 8</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>29220</v>
+        <v>2300</v>
       </c>
       <c r="H21" t="n">
         <v>20</v>
@@ -1101,25 +1101,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D22" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E22" t="n">
         <v>12</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>PCVU 260127 9</t>
+          <t>TWSU 971323 8</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>29000</v>
+        <v>4800</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
@@ -1132,25 +1132,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D23" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E23" t="n">
         <v>12</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>EKCU 260604 6</t>
+          <t>PCTU 351008 5</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>29000</v>
+        <v>32800</v>
       </c>
       <c r="H23" t="n">
         <v>20</v>
@@ -1163,25 +1163,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>107700</v>
+        <v>72000</v>
       </c>
       <c r="D24" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E24" t="n">
         <v>13</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>DHDU 168155 1</t>
+          <t>TKRU 313126 7</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>23294</v>
+        <v>2300</v>
       </c>
       <c r="H24" t="n">
         <v>20</v>
@@ -1194,28 +1194,28 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>107700</v>
+        <v>72000</v>
       </c>
       <c r="D25" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E25" t="n">
         <v>13</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>PCVU 288013 1</t>
+          <t>TCLU 483870 4</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>27000</v>
+        <v>4400</v>
       </c>
       <c r="H25" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I25" t="inlineStr"/>
     </row>
@@ -1225,28 +1225,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>107700</v>
+        <v>92000</v>
       </c>
       <c r="D26" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E26" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>EKCU 260616 0</t>
+          <t>TLLU 158811 1</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>28000</v>
+        <v>26400</v>
       </c>
       <c r="H26" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I26" t="inlineStr"/>
     </row>
@@ -1256,25 +1256,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>107700</v>
+        <v>92000</v>
       </c>
       <c r="D27" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E27" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>EXFU 879643 0</t>
+          <t>NWBU 103506 7</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>29300</v>
+        <v>27800</v>
       </c>
       <c r="H27" t="n">
         <v>20</v>
@@ -1287,28 +1287,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33884962434-5</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>107600</v>
+        <v>92000</v>
       </c>
       <c r="D28" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E28" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>APHU 650279 0</t>
+          <t>PCVU 350020 0</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>8131</v>
+        <v>27920</v>
       </c>
       <c r="H28" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1318,25 +1318,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33884962434-5</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D29" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E29" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>EURU 861007 8</t>
+          <t>MCMU 735118 9</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>29300</v>
+        <v>4800</v>
       </c>
       <c r="H29" t="n">
         <v>20</v>
@@ -1349,25 +1349,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33884962434-5</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D30" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E30" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PCVU 935006 7</t>
+          <t>BTTU 223108 5</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>31800</v>
+        <v>28180</v>
       </c>
       <c r="H30" t="n">
         <v>20</v>
@@ -1380,28 +1380,28 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>107700</v>
+        <v>72000</v>
       </c>
       <c r="D31" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E31" t="n">
         <v>16</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>SEGU 521023 0</t>
+          <t>CAIU 210709 4</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>16938</v>
+        <v>28260</v>
       </c>
       <c r="H31" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I31" t="inlineStr"/>
     </row>
@@ -1411,25 +1411,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D32" t="n">
         <v>90</v>
       </c>
       <c r="E32" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>NWBU 010529 9</t>
+          <t>TKRU 303801 0</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>28000</v>
+        <v>2300</v>
       </c>
       <c r="H32" t="n">
         <v>20</v>
@@ -1442,25 +1442,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D33" t="n">
         <v>90</v>
       </c>
       <c r="E33" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>PAWU 350003 9</t>
+          <t>CAXU 696573 0</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>29800</v>
+        <v>28320</v>
       </c>
       <c r="H33" t="n">
         <v>20</v>
@@ -1473,11 +1473,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D34" t="n">
         <v>90</v>
@@ -1487,11 +1487,11 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>GMCU 238086 6</t>
+          <t>PCVU 935014 9</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>4800</v>
+        <v>31850</v>
       </c>
       <c r="H34" t="n">
         <v>20</v>
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D35" t="n">
         <v>90</v>
@@ -1518,11 +1518,11 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>TKRU 326736 1</t>
+          <t>ABEU 262887 0</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>19634</v>
+        <v>32720</v>
       </c>
       <c r="H35" t="n">
         <v>20</v>
@@ -1535,28 +1535,28 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>107700</v>
+        <v>108000</v>
       </c>
       <c r="D36" t="n">
         <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>PCCU 352602 3</t>
+          <t>NFLU 203462 5</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>31800</v>
+        <v>4500</v>
       </c>
       <c r="H36" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I36" t="inlineStr"/>
     </row>
@@ -1566,28 +1566,28 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>107700</v>
+        <v>108000</v>
       </c>
       <c r="D37" t="n">
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>ABEU 590165 3</t>
+          <t>CLDU 970371 6</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>31300</v>
+        <v>7488</v>
       </c>
       <c r="H37" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I37" t="inlineStr"/>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31804557045-0</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1607,15 +1607,15 @@
         <v>60</v>
       </c>
       <c r="E38" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>EMCU 133658 0</t>
+          <t>NFLU 203458 5</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>15566</v>
+        <v>23500</v>
       </c>
       <c r="H38" t="n">
         <v>40</v>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>31804557045-0</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1638,15 +1638,15 @@
         <v>60</v>
       </c>
       <c r="E39" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TKRU 328147 8</t>
+          <t>PCVU 288022 9</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>19634</v>
+        <v>29280</v>
       </c>
       <c r="H39" t="n">
         <v>20</v>
@@ -1659,28 +1659,28 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D40" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E40" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>CNEU 456619 8</t>
+          <t>TKRU 314169 2</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>9880</v>
+        <v>2300</v>
       </c>
       <c r="H40" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I40" t="inlineStr"/>
     </row>
@@ -1690,25 +1690,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D41" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E41" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TCLU 901180 6</t>
+          <t>BTLU 269021 2</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>27710</v>
+        <v>28090</v>
       </c>
       <c r="H41" t="n">
         <v>20</v>
@@ -1721,25 +1721,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D42" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E42" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>NWBU 010524 1</t>
+          <t>TCKU 133127 8</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>29500</v>
+        <v>28380</v>
       </c>
       <c r="H42" t="n">
         <v>20</v>
@@ -1752,28 +1752,28 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>33684556908-4</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>70000</v>
+        <v>100000</v>
       </c>
       <c r="D43" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E43" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>MCMU 735051 5</t>
+          <t>NFLU 203537 0</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>4800</v>
+        <v>4500</v>
       </c>
       <c r="H43" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I43" t="inlineStr"/>
     </row>
@@ -1783,28 +1783,28 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>33684556908-4</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>70000</v>
+        <v>100000</v>
       </c>
       <c r="D44" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E44" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>CAXU 695595 8</t>
+          <t>CLDU 970465 1</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>28360</v>
+        <v>8660</v>
       </c>
       <c r="H44" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I44" t="inlineStr"/>
     </row>
@@ -1814,25 +1814,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>33684556908-4</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D45" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E45" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>TDTU 058258 0</t>
+          <t>TCKU 345040 3</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>28360</v>
+        <v>25700</v>
       </c>
       <c r="H45" t="n">
         <v>20</v>
@@ -1845,28 +1845,28 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>31804557843-8</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D46" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E46" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>SANU 797461 8</t>
+          <t>ABEU 263315 6</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>9840</v>
+        <v>27600</v>
       </c>
       <c r="H46" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I46" t="inlineStr"/>
     </row>
@@ -1876,185 +1876,30 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>31804557843-8</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D47" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E47" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>EBCU 625052 7</t>
+          <t>TCKU 305135 8</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>31000</v>
+        <v>28620</v>
       </c>
       <c r="H47" t="n">
         <v>20</v>
       </c>
       <c r="I47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>37804557994-3</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D48" t="n">
-        <v>60</v>
-      </c>
-      <c r="E48" t="n">
-        <v>22</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>SANU 751412 4</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>4400</v>
-      </c>
-      <c r="H48" t="n">
-        <v>40</v>
-      </c>
-      <c r="I48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>37804557994-3</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D49" t="n">
-        <v>60</v>
-      </c>
-      <c r="E49" t="n">
-        <v>22</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>NWBU 103525 7</t>
-        </is>
-      </c>
-      <c r="G49" t="n">
-        <v>31800</v>
-      </c>
-      <c r="H49" t="n">
-        <v>20</v>
-      </c>
-      <c r="I49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>37804557177-5</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D50" t="n">
-        <v>60</v>
-      </c>
-      <c r="E50" t="n">
-        <v>23</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>TKRU 303861 6</t>
-        </is>
-      </c>
-      <c r="G50" t="n">
-        <v>2300</v>
-      </c>
-      <c r="H50" t="n">
-        <v>20</v>
-      </c>
-      <c r="I50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>37804557177-5</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D51" t="n">
-        <v>60</v>
-      </c>
-      <c r="E51" t="n">
-        <v>23</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>TRHU 185558 7</t>
-        </is>
-      </c>
-      <c r="G51" t="n">
-        <v>25221</v>
-      </c>
-      <c r="H51" t="n">
-        <v>20</v>
-      </c>
-      <c r="I51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>37804557177-5</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D52" t="n">
-        <v>60</v>
-      </c>
-      <c r="E52" t="n">
-        <v>23</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>CAIU 229409 8</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>28360</v>
-      </c>
-      <c r="H52" t="n">
-        <v>20</v>
-      </c>
-      <c r="I52" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Worked on new model
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,28 +481,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>33544950042-0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>70000</v>
+        <v>92000</v>
       </c>
       <c r="D2" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>TCLU 481269 6</t>
+          <t>PCTU 351010 4</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4400</v>
+        <v>32800</v>
       </c>
       <c r="H2" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I2" t="inlineStr"/>
     </row>
@@ -512,25 +512,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>33544950042-0</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>70000</v>
+        <v>92000</v>
       </c>
       <c r="D3" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MEBU 126421 4</t>
+          <t>ABEU 263266 9</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>28000</v>
+        <v>32440</v>
       </c>
       <c r="H3" t="n">
         <v>20</v>
@@ -543,11 +543,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>33684954257-4</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>108000</v>
+        <v>94000</v>
       </c>
       <c r="D4" t="n">
         <v>90</v>
@@ -557,14 +557,14 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>HMCU 904434 0</t>
+          <t>EURU 405299 6</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>23200</v>
+        <v>2800</v>
       </c>
       <c r="H4" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I4" t="inlineStr"/>
     </row>
@@ -574,11 +574,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>33684954257-4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>108000</v>
+        <v>94000</v>
       </c>
       <c r="D5" t="n">
         <v>90</v>
@@ -588,14 +588,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CLDU 962913 6</t>
+          <t>HOYU 962170 9</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>28836</v>
+        <v>4001</v>
       </c>
       <c r="H5" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -605,28 +605,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>33684954257-4</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>72000</v>
+        <v>94000</v>
       </c>
       <c r="D6" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>TKRU 331851 4</t>
+          <t>TGHU 857827 1</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2300</v>
+        <v>8044</v>
       </c>
       <c r="H6" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I6" t="inlineStr"/>
     </row>
@@ -636,11 +636,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>31804557174-8</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>72000</v>
+        <v>60000</v>
       </c>
       <c r="D7" t="n">
         <v>60</v>
@@ -650,11 +650,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ABEU 260711 5</t>
+          <t>APZU 369950 2</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>25140</v>
+        <v>7770</v>
       </c>
       <c r="H7" t="n">
         <v>20</v>
@@ -667,11 +667,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>31804557174-8</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>72000</v>
+        <v>60000</v>
       </c>
       <c r="D8" t="n">
         <v>60</v>
@@ -681,14 +681,14 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>GCAU 795043 0</t>
+          <t>GESU 642745 8</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>28120</v>
+        <v>13466</v>
       </c>
       <c r="H8" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I8" t="inlineStr"/>
     </row>
@@ -698,25 +698,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>37804557049-6</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D9" t="n">
         <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>GMCU 238079 0</t>
+          <t>FCIU 446212 0</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>4800</v>
+        <v>8000</v>
       </c>
       <c r="H9" t="n">
         <v>20</v>
@@ -729,25 +729,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>37804557049-6</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D10" t="n">
         <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>LYSU 545712 9</t>
+          <t>TGBU 490669 0</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>28386</v>
+        <v>15673</v>
       </c>
       <c r="H10" t="n">
         <v>40</v>
@@ -760,28 +760,28 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33684954286-3</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>107600</v>
+        <v>91000</v>
       </c>
       <c r="D11" t="n">
         <v>90</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>CLDU 961735 1</t>
+          <t>APZU 356204 2</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>8518</v>
+        <v>8647</v>
       </c>
       <c r="H11" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
@@ -791,25 +791,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33684954286-3</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>107600</v>
+        <v>91000</v>
       </c>
       <c r="D12" t="n">
         <v>90</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>NWBU 010529 9</t>
+          <t>BGBU 504706 1</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>28020</v>
+        <v>14000</v>
       </c>
       <c r="H12" t="n">
         <v>20</v>
@@ -822,25 +822,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33684954286-3</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>107600</v>
+        <v>91000</v>
       </c>
       <c r="D13" t="n">
         <v>90</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TANU 351116 0</t>
+          <t>TKRU 325656 2</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>31750</v>
+        <v>19152</v>
       </c>
       <c r="H13" t="n">
         <v>20</v>
@@ -853,25 +853,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33684954286-3</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>70000</v>
+        <v>91000</v>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TKRU 321509 6</t>
+          <t>WEDU 100704 4</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>2300</v>
+        <v>19184</v>
       </c>
       <c r="H14" t="n">
         <v>20</v>
@@ -884,25 +884,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33684557015-7</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D15" t="n">
         <v>60</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ABEU 252405 2</t>
+          <t>WEDU 243552 0</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>27960</v>
+        <v>19184</v>
       </c>
       <c r="H15" t="n">
         <v>20</v>
@@ -915,28 +915,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33684557015-7</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D16" t="n">
         <v>60</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TCLU 226328 3</t>
+          <t>DFSU 677527 8</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>28160</v>
+        <v>23200</v>
       </c>
       <c r="H16" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -946,28 +946,28 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961410-6</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D17" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E17" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>LYSU 546249 1</t>
+          <t>VODU 933849 6</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>28386</v>
+        <v>24800</v>
       </c>
       <c r="H17" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I17" t="inlineStr"/>
     </row>
@@ -977,25 +977,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961410-6</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D18" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ILBU 261007 6</t>
+          <t>ABEU 263034 7</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>28000</v>
+        <v>24440</v>
       </c>
       <c r="H18" t="n">
         <v>20</v>
@@ -1008,28 +1008,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884961410-6</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D19" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E19" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>CMAU 825245 1</t>
+          <t>CMAU 005903 0</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>17011</v>
+        <v>24300</v>
       </c>
       <c r="H19" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1039,25 +1039,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884961410-6</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D20" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E20" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>COUU 810204 9</t>
+          <t>APZU 324940 2</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>32800</v>
+        <v>24300</v>
       </c>
       <c r="H20" t="n">
         <v>20</v>
@@ -1070,25 +1070,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961417-1</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D21" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TKRU 317044 8</t>
+          <t>VTGU 196666 5</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>2300</v>
+        <v>27650</v>
       </c>
       <c r="H21" t="n">
         <v>20</v>
@@ -1101,25 +1101,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961417-1</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D22" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E22" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TWSU 971323 8</t>
+          <t>ABEU 260273 0</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4800</v>
+        <v>27920</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
@@ -1132,25 +1132,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961417-1</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D23" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E23" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>PCTU 351008 5</t>
+          <t>HOYU 241685 2</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>32800</v>
+        <v>28000</v>
       </c>
       <c r="H23" t="n">
         <v>20</v>
@@ -1163,25 +1163,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961369-4</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D24" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E24" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>TKRU 313126 7</t>
+          <t>SAIU 641739 1</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>2300</v>
+        <v>28800</v>
       </c>
       <c r="H24" t="n">
         <v>20</v>
@@ -1194,28 +1194,28 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961369-4</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D25" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E25" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>TCLU 483870 4</t>
+          <t>ABEU 350009 7</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>4400</v>
+        <v>28800</v>
       </c>
       <c r="H25" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I25" t="inlineStr"/>
     </row>
@@ -1225,28 +1225,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884961369-4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>92000</v>
+        <v>108000</v>
       </c>
       <c r="D26" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E26" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TLLU 158811 1</t>
+          <t>ABEU 350005 5</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>26400</v>
+        <v>28800</v>
       </c>
       <c r="H26" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I26" t="inlineStr"/>
     </row>
@@ -1256,25 +1256,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884961350-4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>92000</v>
+        <v>107500</v>
       </c>
       <c r="D27" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E27" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>NWBU 103506 7</t>
+          <t>DHRU 942491 3</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>27800</v>
+        <v>28820</v>
       </c>
       <c r="H27" t="n">
         <v>20</v>
@@ -1287,25 +1287,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884961350-4</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>92000</v>
+        <v>107500</v>
       </c>
       <c r="D28" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E28" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>PCVU 350020 0</t>
+          <t>LAFU 321948 2</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>27920</v>
+        <v>29800</v>
       </c>
       <c r="H28" t="n">
         <v>20</v>
@@ -1318,25 +1318,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33884961350-4</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>72000</v>
+        <v>107500</v>
       </c>
       <c r="D29" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E29" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>MCMU 735118 9</t>
+          <t>CAXU 697533 7</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>4800</v>
+        <v>27600</v>
       </c>
       <c r="H29" t="n">
         <v>20</v>
@@ -1349,28 +1349,28 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33884961070-8</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>72000</v>
+        <v>60000</v>
       </c>
       <c r="D30" t="n">
         <v>60</v>
       </c>
       <c r="E30" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BTTU 223108 5</t>
+          <t>BGFU 972534 6</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>28180</v>
+        <v>26069</v>
       </c>
       <c r="H30" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I30" t="inlineStr"/>
     </row>
@@ -1380,25 +1380,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33884961070-8</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>72000</v>
+        <v>60000</v>
       </c>
       <c r="D31" t="n">
         <v>60</v>
       </c>
       <c r="E31" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>CAIU 210709 4</t>
+          <t>EKCU 360339 7</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>28260</v>
+        <v>33800</v>
       </c>
       <c r="H31" t="n">
         <v>20</v>
@@ -1411,28 +1411,28 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>31804557032-8</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D32" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E32" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>TKRU 303801 0</t>
+          <t>SANU 753011 0</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>2300</v>
+        <v>27148</v>
       </c>
       <c r="H32" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I32" t="inlineStr"/>
     </row>
@@ -1442,25 +1442,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>31804557032-8</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D33" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E33" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>CAXU 696573 0</t>
+          <t>PCVU 261033 1</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>28320</v>
+        <v>29500</v>
       </c>
       <c r="H33" t="n">
         <v>20</v>
@@ -1473,25 +1473,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884962426-1</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>107600</v>
+        <v>108000</v>
       </c>
       <c r="D34" t="n">
         <v>90</v>
       </c>
       <c r="E34" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>PCVU 935014 9</t>
+          <t>SEGU 812764 4</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>31850</v>
+        <v>29520</v>
       </c>
       <c r="H34" t="n">
         <v>20</v>
@@ -1504,25 +1504,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884962426-1</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>107600</v>
+        <v>108000</v>
       </c>
       <c r="D35" t="n">
         <v>90</v>
       </c>
       <c r="E35" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>ABEU 262887 0</t>
+          <t>SEGU 812780 8</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>32720</v>
+        <v>29520</v>
       </c>
       <c r="H35" t="n">
         <v>20</v>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884962426-1</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1545,18 +1545,18 @@
         <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>NFLU 203462 5</t>
+          <t>PCVU 288010 5</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>4500</v>
+        <v>30000</v>
       </c>
       <c r="H36" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I36" t="inlineStr"/>
     </row>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961563-2</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1576,18 +1576,18 @@
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>CLDU 970371 6</t>
+          <t>MTNU 126133 5</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>7488</v>
+        <v>4000</v>
       </c>
       <c r="H37" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I37" t="inlineStr"/>
     </row>
@@ -1597,28 +1597,28 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33884961563-2</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D38" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>NFLU 203458 5</t>
+          <t>GCAU 797129 0</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>23500</v>
+        <v>30800</v>
       </c>
       <c r="H38" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1628,25 +1628,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33884961563-2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D39" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>PCVU 288022 9</t>
+          <t>PCVU 300012 2</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>29280</v>
+        <v>30800</v>
       </c>
       <c r="H39" t="n">
         <v>20</v>
@@ -1659,25 +1659,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33884961563-2</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D40" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E40" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>TKRU 314169 2</t>
+          <t>KRIU 333071 4</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>2300</v>
+        <v>30800</v>
       </c>
       <c r="H40" t="n">
         <v>20</v>
@@ -1690,28 +1690,28 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>37804557212-0</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>70000</v>
+        <v>60000</v>
       </c>
       <c r="D41" t="n">
         <v>60</v>
       </c>
       <c r="E41" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>BTLU 269021 2</t>
+          <t>SANU 750093 8</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>28090</v>
+        <v>27574</v>
       </c>
       <c r="H41" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I41" t="inlineStr"/>
     </row>
@@ -1721,25 +1721,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>37804557212-0</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>70000</v>
+        <v>60000</v>
       </c>
       <c r="D42" t="n">
         <v>60</v>
       </c>
       <c r="E42" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>TCKU 133127 8</t>
+          <t>PCVU 350018 0</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>28380</v>
+        <v>31800</v>
       </c>
       <c r="H42" t="n">
         <v>20</v>
@@ -1752,28 +1752,28 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33684953046-2</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>100000</v>
+        <v>99870</v>
       </c>
       <c r="D43" t="n">
         <v>90</v>
       </c>
       <c r="E43" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>NFLU 203537 0</t>
+          <t>CAIU 257700 9</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>4500</v>
+        <v>28680</v>
       </c>
       <c r="H43" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I43" t="inlineStr"/>
     </row>
@@ -1783,28 +1783,28 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33684953046-2</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>100000</v>
+        <v>99870</v>
       </c>
       <c r="D44" t="n">
         <v>90</v>
       </c>
       <c r="E44" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>CLDU 970465 1</t>
+          <t>PCVU 261048 1</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>8660</v>
+        <v>30500</v>
       </c>
       <c r="H44" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I44" t="inlineStr"/>
     </row>
@@ -1814,25 +1814,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>33684953046-2</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>94000</v>
+        <v>99870</v>
       </c>
       <c r="D45" t="n">
         <v>90</v>
       </c>
       <c r="E45" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>TCKU 345040 3</t>
+          <t>NWBU 050535 6</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>25700</v>
+        <v>29300</v>
       </c>
       <c r="H45" t="n">
         <v>20</v>
@@ -1845,25 +1845,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>37804963044-5</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>94000</v>
+        <v>60000</v>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E46" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>ABEU 263315 6</t>
+          <t>CMAU 323236 5</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>27600</v>
+        <v>24300</v>
       </c>
       <c r="H46" t="n">
         <v>20</v>
@@ -1876,30 +1876,402 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>37804963044-5</t>
         </is>
       </c>
       <c r="C47" t="n">
+        <v>60000</v>
+      </c>
+      <c r="D47" t="n">
+        <v>60</v>
+      </c>
+      <c r="E47" t="n">
+        <v>17</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>ABEU 253211 9</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>34000</v>
+      </c>
+      <c r="H47" t="n">
+        <v>20</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>37804558111-3</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D48" t="n">
+        <v>60</v>
+      </c>
+      <c r="E48" t="n">
+        <v>18</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>PCVU 288004 4</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>31000</v>
+      </c>
+      <c r="H48" t="n">
+        <v>20</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>37804558111-3</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D49" t="n">
+        <v>60</v>
+      </c>
+      <c r="E49" t="n">
+        <v>18</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>TANU 351115 4</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>31800</v>
+      </c>
+      <c r="H49" t="n">
+        <v>20</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>37804850098-7</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>60000</v>
+      </c>
+      <c r="D50" t="n">
+        <v>60</v>
+      </c>
+      <c r="E50" t="n">
+        <v>19</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>ABEU 250113 9</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>34000</v>
+      </c>
+      <c r="H50" t="n">
+        <v>20</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>37804953045-4</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
         <v>94000</v>
       </c>
-      <c r="D47" t="n">
-        <v>90</v>
-      </c>
-      <c r="E47" t="n">
-        <v>24</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>TCKU 305135 8</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
-        <v>28620</v>
-      </c>
-      <c r="H47" t="n">
-        <v>20</v>
-      </c>
-      <c r="I47" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>90</v>
+      </c>
+      <c r="E51" t="n">
+        <v>20</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>TANU 351120 0</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>31800</v>
+      </c>
+      <c r="H51" t="n">
+        <v>20</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>37804953045-4</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>90</v>
+      </c>
+      <c r="E52" t="n">
+        <v>20</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>TANU 351112 8</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>31800</v>
+      </c>
+      <c r="H52" t="n">
+        <v>20</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>37804558117-0</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>60</v>
+      </c>
+      <c r="E53" t="n">
+        <v>21</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>TWSU 271878 9</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>31800</v>
+      </c>
+      <c r="H53" t="n">
+        <v>20</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>37804558117-0</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D54" t="n">
+        <v>60</v>
+      </c>
+      <c r="E54" t="n">
+        <v>21</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>BIDU 497625 8</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>32000</v>
+      </c>
+      <c r="H54" t="n">
+        <v>20</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>33684964208-5</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D55" t="n">
+        <v>90</v>
+      </c>
+      <c r="E55" t="n">
+        <v>22</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>BTLU 269010 4</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>28080</v>
+      </c>
+      <c r="H55" t="n">
+        <v>20</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>33684964208-5</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D56" t="n">
+        <v>90</v>
+      </c>
+      <c r="E56" t="n">
+        <v>22</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>ATRU 330001 0</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>30800</v>
+      </c>
+      <c r="H56" t="n">
+        <v>20</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>33684964208-5</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D57" t="n">
+        <v>90</v>
+      </c>
+      <c r="E57" t="n">
+        <v>22</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>ABEU 263248 4</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>31040</v>
+      </c>
+      <c r="H57" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>37804558159-2</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>60000</v>
+      </c>
+      <c r="D58" t="n">
+        <v>60</v>
+      </c>
+      <c r="E58" t="n">
+        <v>23</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>TCNU 118291 8</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>19087</v>
+      </c>
+      <c r="H58" t="n">
+        <v>40</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>37804558159-2</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>60000</v>
+      </c>
+      <c r="D59" t="n">
+        <v>60</v>
+      </c>
+      <c r="E59" t="n">
+        <v>23</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>ABEU 290005 7</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>34800</v>
+      </c>
+      <c r="H59" t="n">
+        <v>20</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added information to output table in matplotlib
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,25 +481,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>33544950042-0</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>92000</v>
+        <v>70000</v>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PCTU 351010 4</t>
+          <t>TKRU 303801 0</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>32800</v>
+        <v>2300</v>
       </c>
       <c r="H2" t="n">
         <v>20</v>
@@ -512,25 +512,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>33544950042-0</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>92000</v>
+        <v>70000</v>
       </c>
       <c r="D3" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ABEU 263266 9</t>
+          <t>NWBU 050535 6</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>32440</v>
+        <v>28830</v>
       </c>
       <c r="H3" t="n">
         <v>20</v>
@@ -543,30 +543,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>33684954257-4</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>EURU 405299 6</t>
+          <t>TANU 351116 0</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2800</v>
+        <v>31750</v>
       </c>
       <c r="H4" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -574,11 +576,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33684954257-4</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>94000</v>
+        <v>108000</v>
       </c>
       <c r="D5" t="n">
         <v>90</v>
@@ -588,14 +590,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>HOYU 962170 9</t>
+          <t>CMAU 825245 1</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4001</v>
+        <v>17011</v>
       </c>
       <c r="H5" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -605,11 +607,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>33684954257-4</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>94000</v>
+        <v>108000</v>
       </c>
       <c r="D6" t="n">
         <v>90</v>
@@ -619,14 +621,14 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>TGHU 857827 1</t>
+          <t>BTLU 269021 2</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>8044</v>
+        <v>28090</v>
       </c>
       <c r="H6" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I6" t="inlineStr"/>
     </row>
@@ -636,25 +638,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>31804557174-8</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>60000</v>
+        <v>108000</v>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>APZU 369950 2</t>
+          <t>BTTU 223108 5</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>7770</v>
+        <v>28180</v>
       </c>
       <c r="H7" t="n">
         <v>20</v>
@@ -667,11 +669,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31804557174-8</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>60000</v>
+        <v>72000</v>
       </c>
       <c r="D8" t="n">
         <v>60</v>
@@ -681,11 +683,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>GESU 642745 8</t>
+          <t>CLDU 970465 1</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>13466</v>
+        <v>8660</v>
       </c>
       <c r="H8" t="n">
         <v>40</v>
@@ -698,25 +700,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>37804557049-6</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D9" t="n">
         <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>FCIU 446212 0</t>
+          <t>PCVU 260064 7</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>8000</v>
+        <v>29000</v>
       </c>
       <c r="H9" t="n">
         <v>20</v>
@@ -729,25 +731,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>37804557049-6</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D10" t="n">
         <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>TGBU 490669 0</t>
+          <t>HMCU 904434 0</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>15673</v>
+        <v>23200</v>
       </c>
       <c r="H10" t="n">
         <v>40</v>
@@ -760,25 +762,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33684954286-3</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>91000</v>
+        <v>72000</v>
       </c>
       <c r="D11" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>APZU 356204 2</t>
+          <t>PCVU 935014 9</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>8647</v>
+        <v>31850</v>
       </c>
       <c r="H11" t="n">
         <v>20</v>
@@ -791,25 +793,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33684954286-3</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>91000</v>
+        <v>107600</v>
       </c>
       <c r="D12" t="n">
         <v>90</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BGBU 504706 1</t>
+          <t>TKRU 331264 5</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>14000</v>
+        <v>2300</v>
       </c>
       <c r="H12" t="n">
         <v>20</v>
@@ -822,25 +824,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>33684954286-3</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>91000</v>
+        <v>107600</v>
       </c>
       <c r="D13" t="n">
         <v>90</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TKRU 325656 2</t>
+          <t>NWBU 103521 5</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>19152</v>
+        <v>28800</v>
       </c>
       <c r="H13" t="n">
         <v>20</v>
@@ -853,25 +855,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>33684954286-3</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>91000</v>
+        <v>107600</v>
       </c>
       <c r="D14" t="n">
         <v>90</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>WEDU 100704 4</t>
+          <t>NWBU 082664 9</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>19184</v>
+        <v>28880</v>
       </c>
       <c r="H14" t="n">
         <v>20</v>
@@ -884,25 +886,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>33684557015-7</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>WEDU 243552 0</t>
+          <t>MCMU 635042 3</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>19184</v>
+        <v>30040</v>
       </c>
       <c r="H15" t="n">
         <v>20</v>
@@ -915,25 +917,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>33684557015-7</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D16" t="n">
         <v>60</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>DFSU 677527 8</t>
+          <t>TCLU 483870 4</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>23200</v>
+        <v>4400</v>
       </c>
       <c r="H16" t="n">
         <v>40</v>
@@ -946,25 +948,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33884961410-6</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D17" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>VODU 933849 6</t>
+          <t>ILBU 261007 6</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>24800</v>
+        <v>28000</v>
       </c>
       <c r="H17" t="n">
         <v>20</v>
@@ -977,25 +979,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33884961410-6</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D18" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ABEU 263034 7</t>
+          <t>TKRU 313126 7</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>24440</v>
+        <v>2300</v>
       </c>
       <c r="H18" t="n">
         <v>20</v>
@@ -1008,25 +1010,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33884961410-6</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D19" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>CMAU 005903 0</t>
+          <t>COUU 810204 9</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>24300</v>
+        <v>32800</v>
       </c>
       <c r="H19" t="n">
         <v>20</v>
@@ -1039,25 +1041,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33884961410-6</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D20" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>APZU 324940 2</t>
+          <t>ABEU 262887 0</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>24300</v>
+        <v>32720</v>
       </c>
       <c r="H20" t="n">
         <v>20</v>
@@ -1070,25 +1072,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>33884961417-1</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D21" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>VTGU 196666 5</t>
+          <t>TKRU 317044 8</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>27650</v>
+        <v>2300</v>
       </c>
       <c r="H21" t="n">
         <v>20</v>
@@ -1101,30 +1103,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>33884961417-1</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D22" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ABEU 260273 0</t>
+          <t>PCVU 288022 9</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>27920</v>
+        <v>29280</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1132,25 +1136,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33884961417-1</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D23" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>HOYU 241685 2</t>
+          <t>DHDU 208805 2</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>28000</v>
+        <v>29500</v>
       </c>
       <c r="H23" t="n">
         <v>20</v>
@@ -1163,28 +1167,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33884961369-4</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D24" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>SAIU 641739 1</t>
+          <t>TLLU 158811 1</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>28800</v>
+        <v>26400</v>
       </c>
       <c r="H24" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1194,25 +1198,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33884961369-4</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D25" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>ABEU 350009 7</t>
+          <t>ZTKU 735013 0</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>28800</v>
+        <v>31770</v>
       </c>
       <c r="H25" t="n">
         <v>20</v>
@@ -1225,30 +1229,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33884961369-4</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D26" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E26" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ABEU 350005 5</t>
+          <t>TKRU 321509 6</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>28800</v>
+        <v>2300</v>
       </c>
       <c r="H26" t="n">
         <v>20</v>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1256,25 +1262,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>33884961350-4</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>107500</v>
+        <v>72000</v>
       </c>
       <c r="D27" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>DHRU 942491 3</t>
+          <t>PCVU 350020 0</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>28820</v>
+        <v>27920</v>
       </c>
       <c r="H27" t="n">
         <v>20</v>
@@ -1287,30 +1293,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33884961350-4</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>107500</v>
+        <v>72000</v>
       </c>
       <c r="D28" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>LAFU 321948 2</t>
+          <t>MEBU 126421 4</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>29800</v>
+        <v>28000</v>
       </c>
       <c r="H28" t="n">
         <v>20</v>
       </c>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1318,30 +1326,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33884961350-4</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>107500</v>
+        <v>92000</v>
       </c>
       <c r="D29" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>CAXU 697533 7</t>
+          <t>NFLU 203537 0</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>27600</v>
+        <v>4500</v>
       </c>
       <c r="H29" t="n">
-        <v>20</v>
-      </c>
-      <c r="I29" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1349,25 +1359,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33884961070-8</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>60000</v>
+        <v>92000</v>
       </c>
       <c r="D30" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E30" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BGFU 972534 6</t>
+          <t>CLDU 970371 6</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>26069</v>
+        <v>7488</v>
       </c>
       <c r="H30" t="n">
         <v>40</v>
@@ -1380,25 +1390,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>33884961070-8</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>60000</v>
+        <v>72000</v>
       </c>
       <c r="D31" t="n">
         <v>60</v>
       </c>
       <c r="E31" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>EKCU 360339 7</t>
+          <t>ABEU 263315 6</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>33800</v>
+        <v>27600</v>
       </c>
       <c r="H31" t="n">
         <v>20</v>
@@ -1411,7 +1421,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>31804557032-8</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1421,15 +1431,15 @@
         <v>60</v>
       </c>
       <c r="E32" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>SANU 753011 0</t>
+          <t>LYSU 545712 9</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>27148</v>
+        <v>28386</v>
       </c>
       <c r="H32" t="n">
         <v>40</v>
@@ -1442,25 +1452,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>31804557032-8</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D33" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E33" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>PCVU 261033 1</t>
+          <t>MCMU 735118 9</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>29500</v>
+        <v>4800</v>
       </c>
       <c r="H33" t="n">
         <v>20</v>
@@ -1473,28 +1483,28 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33884962426-1</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D34" t="n">
         <v>90</v>
       </c>
       <c r="E34" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>SEGU 812764 4</t>
+          <t>CLDU 961735 1</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>29520</v>
+        <v>8518</v>
       </c>
       <c r="H34" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I34" t="inlineStr"/>
     </row>
@@ -1504,25 +1514,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33884962426-1</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D35" t="n">
         <v>90</v>
       </c>
       <c r="E35" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>SEGU 812780 8</t>
+          <t>TCKU 305135 8</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>29520</v>
+        <v>28620</v>
       </c>
       <c r="H35" t="n">
         <v>20</v>
@@ -1535,7 +1545,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33884962426-1</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1545,15 +1555,15 @@
         <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>PCVU 288010 5</t>
+          <t>TWSU 971323 8</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>30000</v>
+        <v>4800</v>
       </c>
       <c r="H36" t="n">
         <v>20</v>
@@ -1566,7 +1576,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884961563-2</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1576,15 +1586,15 @@
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>MTNU 126133 5</t>
+          <t>GCAU 795043 0</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>4000</v>
+        <v>28120</v>
       </c>
       <c r="H37" t="n">
         <v>20</v>
@@ -1597,7 +1607,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>33884961563-2</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1607,15 +1617,15 @@
         <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>GCAU 797129 0</t>
+          <t>TCLU 226328 3</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>30800</v>
+        <v>28160</v>
       </c>
       <c r="H38" t="n">
         <v>20</v>
@@ -1628,7 +1638,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>33884961563-2</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1638,15 +1648,15 @@
         <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>PCVU 300012 2</t>
+          <t>CAIU 210709 4</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>30800</v>
+        <v>28260</v>
       </c>
       <c r="H39" t="n">
         <v>20</v>
@@ -1659,25 +1669,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>33884961563-2</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D40" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E40" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>KRIU 333071 4</t>
+          <t>GMCU 238079 0</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>30800</v>
+        <v>4800</v>
       </c>
       <c r="H40" t="n">
         <v>20</v>
@@ -1690,25 +1700,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>37804557212-0</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>60000</v>
+        <v>72000</v>
       </c>
       <c r="D41" t="n">
         <v>60</v>
       </c>
       <c r="E41" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>SANU 750093 8</t>
+          <t>TCLU 481269 6</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>27574</v>
+        <v>4400</v>
       </c>
       <c r="H41" t="n">
         <v>40</v>
@@ -1721,25 +1731,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>37804557212-0</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="D42" t="n">
         <v>60</v>
       </c>
       <c r="E42" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>PCVU 350018 0</t>
+          <t>TKRU 331851 4</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>31800</v>
+        <v>2300</v>
       </c>
       <c r="H42" t="n">
         <v>20</v>
@@ -1752,25 +1762,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>33684953046-2</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>99870</v>
+        <v>70000</v>
       </c>
       <c r="D43" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E43" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>CAIU 257700 9</t>
+          <t>ABEU 252405 2</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>28680</v>
+        <v>27960</v>
       </c>
       <c r="H43" t="n">
         <v>20</v>
@@ -1783,25 +1793,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>33684953046-2</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>99870</v>
+        <v>70000</v>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E44" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>PCVU 261048 1</t>
+          <t>NWBU 010529 9</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>30500</v>
+        <v>28020</v>
       </c>
       <c r="H44" t="n">
         <v>20</v>
@@ -1814,28 +1824,28 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>33684953046-2</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>99870</v>
+        <v>100000</v>
       </c>
       <c r="D45" t="n">
         <v>90</v>
       </c>
       <c r="E45" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>NWBU 050535 6</t>
+          <t>CLDU 962913 6</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>29300</v>
+        <v>28836</v>
       </c>
       <c r="H45" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I45" t="inlineStr"/>
     </row>
@@ -1845,25 +1855,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>37804963044-5</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>60000</v>
+        <v>100000</v>
       </c>
       <c r="D46" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E46" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>CMAU 323236 5</t>
+          <t>CAXU 696573 0</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>24300</v>
+        <v>28320</v>
       </c>
       <c r="H46" t="n">
         <v>20</v>
@@ -1876,25 +1886,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>37804963044-5</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>60000</v>
+        <v>100000</v>
       </c>
       <c r="D47" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E47" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>ABEU 253211 9</t>
+          <t>TCKU 133127 8</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>34000</v>
+        <v>28380</v>
       </c>
       <c r="H47" t="n">
         <v>20</v>
@@ -1907,25 +1917,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>37804558111-3</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D48" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E48" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>PCVU 288004 4</t>
+          <t>TKRU 314169 2</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>31000</v>
+        <v>2300</v>
       </c>
       <c r="H48" t="n">
         <v>20</v>
@@ -1938,30 +1948,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>37804558111-3</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D49" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E49" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>TANU 351115 4</t>
+          <t>ABEU 260711 5</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>31800</v>
+        <v>25140</v>
       </c>
       <c r="H49" t="n">
         <v>20</v>
       </c>
-      <c r="I49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1969,25 +1981,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>37804850098-7</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>60000</v>
+        <v>94000</v>
       </c>
       <c r="D50" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E50" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>ABEU 250113 9</t>
+          <t>NWBU 103506 7</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>34000</v>
+        <v>27800</v>
       </c>
       <c r="H50" t="n">
         <v>20</v>
@@ -2000,7 +2012,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>37804953045-4</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -2010,268 +2022,20 @@
         <v>90</v>
       </c>
       <c r="E51" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>TANU 351120 0</t>
+          <t>TCKU 345040 3</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>31800</v>
+        <v>25700</v>
       </c>
       <c r="H51" t="n">
         <v>20</v>
       </c>
       <c r="I51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>37804953045-4</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D52" t="n">
-        <v>90</v>
-      </c>
-      <c r="E52" t="n">
-        <v>20</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>TANU 351112 8</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>31800</v>
-      </c>
-      <c r="H52" t="n">
-        <v>20</v>
-      </c>
-      <c r="I52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>37804558117-0</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D53" t="n">
-        <v>60</v>
-      </c>
-      <c r="E53" t="n">
-        <v>21</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>TWSU 271878 9</t>
-        </is>
-      </c>
-      <c r="G53" t="n">
-        <v>31800</v>
-      </c>
-      <c r="H53" t="n">
-        <v>20</v>
-      </c>
-      <c r="I53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>37804558117-0</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D54" t="n">
-        <v>60</v>
-      </c>
-      <c r="E54" t="n">
-        <v>21</v>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>BIDU 497625 8</t>
-        </is>
-      </c>
-      <c r="G54" t="n">
-        <v>32000</v>
-      </c>
-      <c r="H54" t="n">
-        <v>20</v>
-      </c>
-      <c r="I54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>33684964208-5</t>
-        </is>
-      </c>
-      <c r="C55" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D55" t="n">
-        <v>90</v>
-      </c>
-      <c r="E55" t="n">
-        <v>22</v>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>BTLU 269010 4</t>
-        </is>
-      </c>
-      <c r="G55" t="n">
-        <v>28080</v>
-      </c>
-      <c r="H55" t="n">
-        <v>20</v>
-      </c>
-      <c r="I55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>33684964208-5</t>
-        </is>
-      </c>
-      <c r="C56" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D56" t="n">
-        <v>90</v>
-      </c>
-      <c r="E56" t="n">
-        <v>22</v>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>ATRU 330001 0</t>
-        </is>
-      </c>
-      <c r="G56" t="n">
-        <v>30800</v>
-      </c>
-      <c r="H56" t="n">
-        <v>20</v>
-      </c>
-      <c r="I56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>33684964208-5</t>
-        </is>
-      </c>
-      <c r="C57" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D57" t="n">
-        <v>90</v>
-      </c>
-      <c r="E57" t="n">
-        <v>22</v>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>ABEU 263248 4</t>
-        </is>
-      </c>
-      <c r="G57" t="n">
-        <v>31040</v>
-      </c>
-      <c r="H57" t="n">
-        <v>20</v>
-      </c>
-      <c r="I57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>37804558159-2</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>60000</v>
-      </c>
-      <c r="D58" t="n">
-        <v>60</v>
-      </c>
-      <c r="E58" t="n">
-        <v>23</v>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>TCNU 118291 8</t>
-        </is>
-      </c>
-      <c r="G58" t="n">
-        <v>19087</v>
-      </c>
-      <c r="H58" t="n">
-        <v>40</v>
-      </c>
-      <c r="I58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>37804558159-2</t>
-        </is>
-      </c>
-      <c r="C59" t="n">
-        <v>60000</v>
-      </c>
-      <c r="D59" t="n">
-        <v>60</v>
-      </c>
-      <c r="E59" t="n">
-        <v>23</v>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>ABEU 290005 7</t>
-        </is>
-      </c>
-      <c r="G59" t="n">
-        <v>34800</v>
-      </c>
-      <c r="H59" t="n">
-        <v>20</v>
-      </c>
-      <c r="I59" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Optimal axle load looked for after finding solution
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,16 +495,18 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>TKRU 303801 0</t>
+          <t>PCVU 288022 9</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2300</v>
+        <v>29280</v>
       </c>
       <c r="H2" t="n">
         <v>20</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -526,11 +528,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>NWBU 050535 6</t>
+          <t>TKRU 313126 7</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>28830</v>
+        <v>2300</v>
       </c>
       <c r="H3" t="n">
         <v>20</v>
@@ -590,14 +592,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CMAU 825245 1</t>
+          <t>TKRU 317044 8</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>17011</v>
+        <v>2300</v>
       </c>
       <c r="H5" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -621,16 +623,18 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BTLU 269021 2</t>
+          <t>MEBU 126421 4</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>28090</v>
+        <v>28000</v>
       </c>
       <c r="H6" t="n">
         <v>20</v>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -652,14 +656,14 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>BTTU 223108 5</t>
+          <t>CLDU 962913 6</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>28180</v>
+        <v>28836</v>
       </c>
       <c r="H7" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -669,28 +673,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>CLDU 970465 1</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>8660</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I8" t="inlineStr"/>
     </row>
@@ -700,28 +704,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>PCVU 260064 7</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>29000</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -731,7 +735,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -741,19 +745,11 @@
         <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>HMCU 904434 0</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>23200</v>
-      </c>
-      <c r="H10" t="n">
-        <v>40</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -776,16 +772,18 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PCVU 935014 9</t>
+          <t>ABEU 260711 5</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>31850</v>
+        <v>25140</v>
       </c>
       <c r="H11" t="n">
         <v>20</v>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -793,28 +791,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D12" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>TKRU 331264 5</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>2300</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -824,28 +822,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D13" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>NWBU 103521 5</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>28800</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -855,25 +853,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>NWBU 082664 9</t>
+          <t>TCKU 345040 3</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>28880</v>
+        <v>25700</v>
       </c>
       <c r="H14" t="n">
         <v>20</v>
@@ -900,11 +898,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>MCMU 635042 3</t>
+          <t>TKRU 331264 5</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>30040</v>
+        <v>2300</v>
       </c>
       <c r="H15" t="n">
         <v>20</v>
@@ -917,25 +915,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D16" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TCLU 483870 4</t>
+          <t>LYSU 545712 9</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>4400</v>
+        <v>28386</v>
       </c>
       <c r="H16" t="n">
         <v>40</v>
@@ -948,25 +946,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D17" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ILBU 261007 6</t>
+          <t>ABEU 252405 2</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>28000</v>
+        <v>27960</v>
       </c>
       <c r="H17" t="n">
         <v>20</v>
@@ -979,28 +977,28 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D18" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>TKRU 313126 7</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>2300</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I18" t="inlineStr"/>
     </row>
@@ -1010,28 +1008,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D19" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>COUU 810204 9</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>32800</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1041,7 +1039,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1051,15 +1049,15 @@
         <v>60</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>ABEU 262887 0</t>
+          <t>TKRU 314169 2</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>32720</v>
+        <v>2300</v>
       </c>
       <c r="H20" t="n">
         <v>20</v>
@@ -1072,28 +1070,28 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D21" t="n">
         <v>60</v>
       </c>
       <c r="E21" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TKRU 317044 8</t>
+          <t>LYSU 546249 1</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>2300</v>
+        <v>28386</v>
       </c>
       <c r="H21" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>
@@ -1103,32 +1101,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D22" t="n">
         <v>60</v>
       </c>
       <c r="E22" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>PCVU 288022 9</t>
+          <t>ABEU 263315 6</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>29280</v>
+        <v>27600</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
       </c>
-      <c r="I22" t="n">
-        <v>1</v>
-      </c>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1136,25 +1132,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D23" t="n">
         <v>60</v>
       </c>
       <c r="E23" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>DHDU 208805 2</t>
+          <t>TKRU 331851 4</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>29500</v>
+        <v>2300</v>
       </c>
       <c r="H23" t="n">
         <v>20</v>
@@ -1167,28 +1163,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D24" t="n">
         <v>60</v>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>TLLU 158811 1</t>
+          <t>PCVU 350020 0</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>26400</v>
+        <v>27920</v>
       </c>
       <c r="H24" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1198,7 +1194,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1208,18 +1204,18 @@
         <v>60</v>
       </c>
       <c r="E25" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>ZTKU 735013 0</t>
+          <t>CMAU 825245 1</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>31770</v>
+        <v>17011</v>
       </c>
       <c r="H25" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I25" t="inlineStr"/>
     </row>
@@ -1229,7 +1225,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1239,22 +1235,20 @@
         <v>60</v>
       </c>
       <c r="E26" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TKRU 321509 6</t>
+          <t>NWBU 103506 7</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>2300</v>
+        <v>27800</v>
       </c>
       <c r="H26" t="n">
         <v>20</v>
       </c>
-      <c r="I26" t="n">
-        <v>1</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1262,7 +1256,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1272,18 +1266,18 @@
         <v>60</v>
       </c>
       <c r="E27" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>PCVU 350020 0</t>
+          <t>CLDU 970371 6</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>27920</v>
+        <v>7488</v>
       </c>
       <c r="H27" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1293,7 +1287,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1303,22 +1297,20 @@
         <v>60</v>
       </c>
       <c r="E28" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>MEBU 126421 4</t>
+          <t>MCMU 735118 9</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>28000</v>
+        <v>4800</v>
       </c>
       <c r="H28" t="n">
         <v>20</v>
       </c>
-      <c r="I28" t="n">
-        <v>1</v>
-      </c>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1326,32 +1318,30 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>92000</v>
+        <v>72000</v>
       </c>
       <c r="D29" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E29" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>NFLU 203537 0</t>
+          <t>TKRU 303801 0</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>4500</v>
+        <v>2300</v>
       </c>
       <c r="H29" t="n">
-        <v>40</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1359,25 +1349,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>92000</v>
+        <v>72000</v>
       </c>
       <c r="D30" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E30" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>CLDU 970371 6</t>
+          <t>CLDU 961735 1</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>7488</v>
+        <v>8518</v>
       </c>
       <c r="H30" t="n">
         <v>40</v>
@@ -1390,28 +1380,28 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>72000</v>
+        <v>92000</v>
       </c>
       <c r="D31" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E31" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ABEU 263315 6</t>
+          <t>NFLU 203462 5</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>27600</v>
+        <v>4500</v>
       </c>
       <c r="H31" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I31" t="inlineStr"/>
     </row>
@@ -1421,25 +1411,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>72000</v>
+        <v>92000</v>
       </c>
       <c r="D32" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E32" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>LYSU 545712 9</t>
+          <t>TCLU 483870 4</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>28386</v>
+        <v>4400</v>
       </c>
       <c r="H32" t="n">
         <v>40</v>
@@ -1452,25 +1442,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D33" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E33" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>MCMU 735118 9</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>4800</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
         <v>20</v>
@@ -1483,30 +1473,32 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D34" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E34" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>CLDU 961735 1</t>
+          <t>TKRU 321509 6</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>8518</v>
+        <v>2300</v>
       </c>
       <c r="H34" t="n">
-        <v>40</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1514,25 +1506,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D35" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E35" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>TCKU 305135 8</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>28620</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
         <v>20</v>
@@ -1545,30 +1537,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D36" t="n">
         <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>TWSU 971323 8</t>
+          <t>NFLU 203537 0</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>4800</v>
+        <v>4500</v>
       </c>
       <c r="H36" t="n">
-        <v>20</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1576,28 +1570,28 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D37" t="n">
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>GCAU 795043 0</t>
+          <t>TCLU 481269 6</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>28120</v>
+        <v>4400</v>
       </c>
       <c r="H37" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I37" t="inlineStr"/>
     </row>
@@ -1607,28 +1601,28 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D38" t="n">
         <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>TCLU 226328 3</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>28160</v>
+        <v>1</v>
       </c>
       <c r="H38" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1638,28 +1632,28 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D39" t="n">
         <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>CAIU 210709 4</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>28260</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I39" t="inlineStr"/>
     </row>
@@ -1669,28 +1663,28 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D40" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E40" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>GMCU 238079 0</t>
+          <t>HMCU 904434 0</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>4800</v>
+        <v>23200</v>
       </c>
       <c r="H40" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I40" t="inlineStr"/>
     </row>
@@ -1700,25 +1694,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D41" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E41" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TCLU 481269 6</t>
+          <t>NFLU 203458 5</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4400</v>
+        <v>23500</v>
       </c>
       <c r="H41" t="n">
         <v>40</v>
@@ -1731,28 +1725,28 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D42" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E42" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>TKRU 331851 4</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>2300</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I42" t="inlineStr"/>
     </row>
@@ -1762,28 +1756,28 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D43" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E43" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>ABEU 252405 2</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>27960</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I43" t="inlineStr"/>
     </row>
@@ -1793,28 +1787,28 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D44" t="n">
         <v>60</v>
       </c>
       <c r="E44" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>NWBU 010529 9</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>28020</v>
+        <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I44" t="inlineStr"/>
     </row>
@@ -1824,28 +1818,28 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>100000</v>
+        <v>72000</v>
       </c>
       <c r="D45" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E45" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>CLDU 962913 6</t>
+          <t>TWSU 971323 8</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>28836</v>
+        <v>4800</v>
       </c>
       <c r="H45" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I45" t="inlineStr"/>
     </row>
@@ -1855,25 +1849,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>100000</v>
+        <v>72000</v>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E46" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>CAXU 696573 0</t>
+          <t>GMCU 238079 0</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>28320</v>
+        <v>4800</v>
       </c>
       <c r="H46" t="n">
         <v>20</v>
@@ -1886,28 +1880,28 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>100000</v>
+        <v>72000</v>
       </c>
       <c r="D47" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E47" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>TCKU 133127 8</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>28380</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I47" t="inlineStr"/>
     </row>
@@ -1917,29 +1911,21 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D48" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E48" t="n">
-        <v>24</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>TKRU 314169 2</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>2300</v>
-      </c>
-      <c r="H48" t="n">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
@@ -1948,32 +1934,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>94000</v>
+        <v>100000</v>
       </c>
       <c r="D49" t="n">
         <v>90</v>
       </c>
       <c r="E49" t="n">
-        <v>24</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>ABEU 260711 5</t>
-        </is>
-      </c>
-      <c r="G49" t="n">
-        <v>25140</v>
-      </c>
-      <c r="H49" t="n">
-        <v>20</v>
-      </c>
-      <c r="I49" t="n">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1995,14 +1971,14 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>NWBU 103506 7</t>
+          <t>CLDU 970465 1</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>27800</v>
+        <v>8660</v>
       </c>
       <c r="H50" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I50" t="inlineStr"/>
     </row>
@@ -2026,16 +2002,78 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>TCKU 345040 3</t>
+          <t>TLLU 158811 1</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>25700</v>
+        <v>26400</v>
       </c>
       <c r="H51" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>90</v>
+      </c>
+      <c r="E52" t="n">
+        <v>24</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>DUMMY1</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="n">
+        <v>5</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>90</v>
+      </c>
+      <c r="E53" t="n">
+        <v>24</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>DUMMY2</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
All wagon if there are enough containers
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,20 +493,10 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>PCVU 288022 9</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>29280</v>
-      </c>
-      <c r="H2" t="n">
-        <v>20</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -514,29 +504,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D3" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>TKRU 313126 7</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>2300</v>
-      </c>
-      <c r="H3" t="n">
-        <v>20</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -545,32 +527,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D4" t="n">
         <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>TANU 351116 0</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>31750</v>
-      </c>
-      <c r="H4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -578,28 +550,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TKRU 317044 8</t>
+          <t>NFLU 203462 5</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2300</v>
+        <v>4500</v>
       </c>
       <c r="H5" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -609,32 +581,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D6" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MEBU 126421 4</t>
+          <t>TKRU 314169 2</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>28000</v>
+        <v>2300</v>
       </c>
       <c r="H6" t="n">
         <v>20</v>
       </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -642,25 +612,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D7" t="n">
         <v>90</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CLDU 962913 6</t>
+          <t>CLDU 970371 6</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>28836</v>
+        <v>7488</v>
       </c>
       <c r="H7" t="n">
         <v>40</v>
@@ -673,30 +643,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D8" t="n">
         <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>TKRU 321509 6</t>
         </is>
       </c>
       <c r="G8" t="n">
+        <v>2300</v>
+      </c>
+      <c r="H8" t="n">
+        <v>20</v>
+      </c>
+      <c r="I8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
-        <v>5</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -704,28 +676,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>108000</v>
+        <v>107600</v>
       </c>
       <c r="D9" t="n">
         <v>90</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>TKRU 331851 4</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>2300</v>
       </c>
       <c r="H9" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -735,22 +707,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D10" t="n">
         <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NFLU 203537 0</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>4500</v>
+      </c>
+      <c r="H10" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -758,32 +740,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D11" t="n">
         <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>ABEU 260711 5</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>25140</v>
-      </c>
-      <c r="H11" t="n">
-        <v>20</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -791,7 +763,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -801,18 +773,18 @@
         <v>60</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>TKRU 313126 7</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>2300</v>
       </c>
       <c r="H12" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -822,7 +794,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -832,18 +804,18 @@
         <v>60</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>CLDU 970465 1</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>8660</v>
       </c>
       <c r="H13" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -853,7 +825,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -863,18 +835,18 @@
         <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TCKU 345040 3</t>
+          <t>TCLU 481269 6</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>25700</v>
+        <v>4400</v>
       </c>
       <c r="H14" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -884,29 +856,21 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D15" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>TKRU 331264 5</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>2300</v>
-      </c>
-      <c r="H15" t="n">
-        <v>20</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -915,25 +879,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>107600</v>
+        <v>92000</v>
       </c>
       <c r="D16" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>LYSU 545712 9</t>
+          <t>TCLU 483870 4</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>28386</v>
+        <v>4400</v>
       </c>
       <c r="H16" t="n">
         <v>40</v>
@@ -946,25 +910,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>107600</v>
+        <v>92000</v>
       </c>
       <c r="D17" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ABEU 252405 2</t>
+          <t>TKRU 303801 0</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>27960</v>
+        <v>2300</v>
       </c>
       <c r="H17" t="n">
         <v>20</v>
@@ -977,29 +941,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D18" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>DUMMY1</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" t="n">
-        <v>5</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -1008,7 +964,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1018,18 +974,18 @@
         <v>90</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>MCMU 735118 9</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>1</v>
+        <v>4800</v>
       </c>
       <c r="H19" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1039,25 +995,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D20" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TKRU 314169 2</t>
+          <t>GMCU 238079 0</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>2300</v>
+        <v>4800</v>
       </c>
       <c r="H20" t="n">
         <v>20</v>
@@ -1070,28 +1026,28 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D21" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>LYSU 546249 1</t>
+          <t>NWBU 103506 7</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>28386</v>
+        <v>27800</v>
       </c>
       <c r="H21" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>
@@ -1101,25 +1057,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D22" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ABEU 263315 6</t>
+          <t>PCVU 350020 0</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>27600</v>
+        <v>27920</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
@@ -1132,28 +1088,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D23" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>TKRU 331851 4</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>2300</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I23" t="inlineStr"/>
     </row>
@@ -1163,28 +1119,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D24" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PCVU 350020 0</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>27920</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1194,25 +1150,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D25" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E25" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>CMAU 825245 1</t>
+          <t>CLDU 961735 1</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>17011</v>
+        <v>8518</v>
       </c>
       <c r="H25" t="n">
         <v>40</v>
@@ -1225,30 +1181,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D26" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E26" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>NWBU 103506 7</t>
+          <t>ABEU 260711 5</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>27800</v>
+        <v>25140</v>
       </c>
       <c r="H26" t="n">
         <v>20</v>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1256,28 +1214,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D27" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E27" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>CLDU 970371 6</t>
+          <t>TCKU 345040 3</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>7488</v>
+        <v>25700</v>
       </c>
       <c r="H27" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1287,28 +1245,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D28" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E28" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>MCMU 735118 9</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>4800</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1318,28 +1276,28 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961020-3</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D29" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E29" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>TKRU 303801 0</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>2300</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I29" t="inlineStr"/>
     </row>
@@ -1349,7 +1307,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>31804557039-3</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1359,19 +1317,11 @@
         <v>60</v>
       </c>
       <c r="E30" t="n">
-        <v>13</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>CLDU 961735 1</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
-        <v>8518</v>
-      </c>
-      <c r="H30" t="n">
-        <v>40</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -1380,28 +1330,28 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>92000</v>
+        <v>70000</v>
       </c>
       <c r="D31" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E31" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>NFLU 203462 5</t>
+          <t>TWSU 971323 8</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>4500</v>
+        <v>4800</v>
       </c>
       <c r="H31" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I31" t="inlineStr"/>
     </row>
@@ -1411,25 +1361,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>37804557179-1</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>92000</v>
+        <v>70000</v>
       </c>
       <c r="D32" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E32" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>TCLU 483870 4</t>
+          <t>HMCU 904434 0</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>4400</v>
+        <v>23200</v>
       </c>
       <c r="H32" t="n">
         <v>40</v>
@@ -1442,25 +1392,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>72000</v>
+        <v>100000</v>
       </c>
       <c r="D33" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E33" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>TKRU 317044 8</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>2300</v>
       </c>
       <c r="H33" t="n">
         <v>20</v>
@@ -1473,21 +1423,21 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>72000</v>
+        <v>100000</v>
       </c>
       <c r="D34" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E34" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>TKRU 321509 6</t>
+          <t>TKRU 331264 5</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1496,9 +1446,7 @@
       <c r="H34" t="n">
         <v>20</v>
       </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1506,28 +1454,28 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>72000</v>
+        <v>100000</v>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E35" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>NFLU 203458 5</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>23500</v>
       </c>
       <c r="H35" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I35" t="inlineStr"/>
     </row>
@@ -1537,32 +1485,30 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>107600</v>
+        <v>100000</v>
       </c>
       <c r="D36" t="n">
         <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>NFLU 203537 0</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>4500</v>
+        <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>40</v>
-      </c>
-      <c r="I36" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1570,28 +1516,28 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684953049-6</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>107600</v>
+        <v>100000</v>
       </c>
       <c r="D37" t="n">
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>TCLU 481269 6</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>4400</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I37" t="inlineStr"/>
     </row>
@@ -1601,28 +1547,28 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>107600</v>
+        <v>94000</v>
       </c>
       <c r="D38" t="n">
         <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>CMAU 825245 1</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>17011</v>
       </c>
       <c r="H38" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1632,28 +1578,28 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>107600</v>
+        <v>94000</v>
       </c>
       <c r="D39" t="n">
         <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>TLLU 158811 1</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>26400</v>
       </c>
       <c r="H39" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I39" t="inlineStr"/>
     </row>
@@ -1663,28 +1609,28 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>108000</v>
+        <v>94000</v>
       </c>
       <c r="D40" t="n">
         <v>90</v>
       </c>
       <c r="E40" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>HMCU 904434 0</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>23200</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I40" t="inlineStr"/>
     </row>
@@ -1694,386 +1640,30 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>37804952303-8</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>108000</v>
+        <v>94000</v>
       </c>
       <c r="D41" t="n">
         <v>90</v>
       </c>
       <c r="E41" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>NFLU 203458 5</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>23500</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>33884961020-3</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>108000</v>
-      </c>
-      <c r="D42" t="n">
-        <v>90</v>
-      </c>
-      <c r="E42" t="n">
-        <v>18</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>DUMMY1</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" t="n">
-        <v>5</v>
-      </c>
-      <c r="I42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>33884961020-3</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>108000</v>
-      </c>
-      <c r="D43" t="n">
-        <v>90</v>
-      </c>
-      <c r="E43" t="n">
-        <v>18</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>DUMMY2</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" t="n">
-        <v>5</v>
-      </c>
-      <c r="I43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>31804557039-3</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>72000</v>
-      </c>
-      <c r="D44" t="n">
-        <v>60</v>
-      </c>
-      <c r="E44" t="n">
-        <v>21</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>DUMMY1</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" t="n">
-        <v>10</v>
-      </c>
-      <c r="I44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>31804557039-3</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>72000</v>
-      </c>
-      <c r="D45" t="n">
-        <v>60</v>
-      </c>
-      <c r="E45" t="n">
-        <v>21</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>TWSU 971323 8</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
-        <v>4800</v>
-      </c>
-      <c r="H45" t="n">
-        <v>20</v>
-      </c>
-      <c r="I45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>31804557039-3</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>72000</v>
-      </c>
-      <c r="D46" t="n">
-        <v>60</v>
-      </c>
-      <c r="E46" t="n">
-        <v>21</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>GMCU 238079 0</t>
-        </is>
-      </c>
-      <c r="G46" t="n">
-        <v>4800</v>
-      </c>
-      <c r="H46" t="n">
-        <v>20</v>
-      </c>
-      <c r="I46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>31804557039-3</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
-        <v>72000</v>
-      </c>
-      <c r="D47" t="n">
-        <v>60</v>
-      </c>
-      <c r="E47" t="n">
-        <v>21</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>DUMMY2</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H47" t="n">
-        <v>10</v>
-      </c>
-      <c r="I47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>37804557179-1</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>70000</v>
-      </c>
-      <c r="D48" t="n">
-        <v>60</v>
-      </c>
-      <c r="E48" t="n">
-        <v>22</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>33684953049-6</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>100000</v>
-      </c>
-      <c r="D49" t="n">
-        <v>90</v>
-      </c>
-      <c r="E49" t="n">
-        <v>23</v>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D50" t="n">
-        <v>90</v>
-      </c>
-      <c r="E50" t="n">
-        <v>24</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>CLDU 970465 1</t>
-        </is>
-      </c>
-      <c r="G50" t="n">
-        <v>8660</v>
-      </c>
-      <c r="H50" t="n">
-        <v>40</v>
-      </c>
-      <c r="I50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D51" t="n">
-        <v>90</v>
-      </c>
-      <c r="E51" t="n">
-        <v>24</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>TLLU 158811 1</t>
-        </is>
-      </c>
-      <c r="G51" t="n">
-        <v>26400</v>
-      </c>
-      <c r="H51" t="n">
-        <v>40</v>
-      </c>
-      <c r="I51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D52" t="n">
-        <v>90</v>
-      </c>
-      <c r="E52" t="n">
-        <v>24</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>DUMMY1</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" t="n">
-        <v>5</v>
-      </c>
-      <c r="I52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D53" t="n">
-        <v>90</v>
-      </c>
-      <c r="E53" t="n">
-        <v>24</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>DUMMY2</t>
-        </is>
-      </c>
-      <c r="G53" t="n">
-        <v>1</v>
-      </c>
-      <c r="H53" t="n">
-        <v>5</v>
-      </c>
-      <c r="I53" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Empty Space is visible again
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,9 +493,17 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NWBU 050535 6</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>28830</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
       <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -504,21 +512,29 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D3" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>TKRU 303801 0</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>2300</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
       <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -527,22 +543,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>37804556544-7</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D4" t="n">
         <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>TANU 351116 0</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>31750</v>
+      </c>
+      <c r="H4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -550,28 +576,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D5" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NFLU 203462 5</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4500</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -581,25 +607,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D6" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>TKRU 314169 2</t>
+          <t>BTTU 223108 5</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2300</v>
+        <v>28180</v>
       </c>
       <c r="H6" t="n">
         <v>20</v>
@@ -612,28 +638,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>107600</v>
+        <v>108000</v>
       </c>
       <c r="D7" t="n">
         <v>90</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CLDU 970371 6</t>
+          <t>DUMMY2</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>7488</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -643,32 +669,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>107600</v>
+        <v>108000</v>
       </c>
       <c r="D8" t="n">
         <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TKRU 321509 6</t>
+          <t>CMAU 825245 1</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2300</v>
+        <v>17011</v>
       </c>
       <c r="H8" t="n">
-        <v>20</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -676,25 +700,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>33884962390-9</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>107600</v>
+        <v>108000</v>
       </c>
       <c r="D9" t="n">
         <v>90</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>TKRU 331851 4</t>
+          <t>BTLU 269021 2</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>2300</v>
+        <v>28090</v>
       </c>
       <c r="H9" t="n">
         <v>20</v>
@@ -707,32 +731,30 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D10" t="n">
         <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>NFLU 203537 0</t>
+          <t>CLDU 970465 1</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>4500</v>
+        <v>8660</v>
       </c>
       <c r="H10" t="n">
         <v>40</v>
       </c>
-      <c r="I10" t="n">
-        <v>1</v>
-      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -740,21 +762,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>31804557008-8</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D11" t="n">
         <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>9</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>PCVU 260064 7</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>29000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>20</v>
+      </c>
       <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -763,7 +793,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -773,18 +803,18 @@
         <v>60</v>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>TKRU 313126 7</t>
+          <t>HMCU 904434 0</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>2300</v>
+        <v>23200</v>
       </c>
       <c r="H12" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -794,7 +824,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>31804557021-1</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -804,18 +834,18 @@
         <v>60</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>CLDU 970465 1</t>
+          <t>PCVU 935014 9</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>8660</v>
+        <v>31850</v>
       </c>
       <c r="H13" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -825,28 +855,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D14" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TCLU 481269 6</t>
+          <t>MCMU 635042 3</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>4400</v>
+        <v>30040</v>
       </c>
       <c r="H14" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -856,21 +886,29 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D15" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>TKRU 331264 5</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>2300</v>
+      </c>
+      <c r="H15" t="n">
+        <v>20</v>
+      </c>
       <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -879,28 +917,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>92000</v>
+        <v>107600</v>
       </c>
       <c r="D16" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E16" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TCLU 483870 4</t>
+          <t>DUMMY1</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>4400</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -910,25 +948,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>92000</v>
+        <v>107600</v>
       </c>
       <c r="D17" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E17" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>TKRU 303801 0</t>
+          <t>NWBU 082664 9</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>2300</v>
+        <v>28880</v>
       </c>
       <c r="H17" t="n">
         <v>20</v>
@@ -941,21 +979,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D18" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E18" t="n">
-        <v>16</v>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>DUMMY2</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>5</v>
+      </c>
       <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -964,7 +1010,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884961594-7</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -974,15 +1020,15 @@
         <v>90</v>
       </c>
       <c r="E19" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>MCMU 735118 9</t>
+          <t>NWBU 103521 5</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>4800</v>
+        <v>28800</v>
       </c>
       <c r="H19" t="n">
         <v>20</v>
@@ -995,28 +1041,28 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D20" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E20" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>GMCU 238079 0</t>
+          <t>TCLU 483870 4</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>4800</v>
+        <v>4400</v>
       </c>
       <c r="H20" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I20" t="inlineStr"/>
     </row>
@@ -1026,25 +1072,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684556915-9</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D21" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E21" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>NWBU 103506 7</t>
+          <t>ILBU 261007 6</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>27800</v>
+        <v>28000</v>
       </c>
       <c r="H21" t="n">
         <v>20</v>
@@ -1057,25 +1103,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D22" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E22" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>PCVU 350020 0</t>
+          <t>ABEU 262887 0</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>27920</v>
+        <v>32720</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
@@ -1088,28 +1134,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D23" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E23" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>TKRU 313126 7</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>2300</v>
       </c>
       <c r="H23" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I23" t="inlineStr"/>
     </row>
@@ -1119,28 +1165,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33684556912-6</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D24" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E24" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>COUU 810204 9</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>32800</v>
       </c>
       <c r="H24" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1150,30 +1196,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D25" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E25" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>CLDU 961735 1</t>
+          <t>PCVU 288022 9</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>8518</v>
+        <v>29280</v>
       </c>
       <c r="H25" t="n">
-        <v>40</v>
-      </c>
-      <c r="I25" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1181,32 +1229,30 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D26" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E26" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ABEU 260711 5</t>
+          <t>TKRU 317044 8</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>25140</v>
+        <v>2300</v>
       </c>
       <c r="H26" t="n">
         <v>20</v>
       </c>
-      <c r="I26" t="n">
-        <v>1</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1214,25 +1260,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557042-7</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D27" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E27" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>TCKU 345040 3</t>
+          <t>DHDU 208805 2</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>25700</v>
+        <v>29500</v>
       </c>
       <c r="H27" t="n">
         <v>20</v>
@@ -1245,28 +1291,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D28" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E28" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>TLLU 158811 1</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>26400</v>
       </c>
       <c r="H28" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1276,28 +1322,28 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557059-1</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D29" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E29" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>ZTKU 735013 0</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>31770</v>
       </c>
       <c r="H29" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I29" t="inlineStr"/>
     </row>
@@ -1307,7 +1353,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1317,11 +1363,19 @@
         <v>60</v>
       </c>
       <c r="E30" t="n">
-        <v>21</v>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>PCVU 350020 0</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>27920</v>
+      </c>
+      <c r="H30" t="n">
+        <v>20</v>
+      </c>
       <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -1330,30 +1384,32 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D31" t="n">
         <v>60</v>
       </c>
       <c r="E31" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TWSU 971323 8</t>
+          <t>TKRU 321509 6</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>4800</v>
+        <v>2300</v>
       </c>
       <c r="H31" t="n">
         <v>20</v>
       </c>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1361,30 +1417,32 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33684556890-4</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D32" t="n">
         <v>60</v>
       </c>
       <c r="E32" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>HMCU 904434 0</t>
+          <t>MEBU 126421 4</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>23200</v>
+        <v>28000</v>
       </c>
       <c r="H32" t="n">
-        <v>40</v>
-      </c>
-      <c r="I32" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1392,28 +1450,28 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>100000</v>
+        <v>92000</v>
       </c>
       <c r="D33" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E33" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TKRU 317044 8</t>
+          <t>CLDU 970371 6</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>2300</v>
+        <v>7488</v>
       </c>
       <c r="H33" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I33" t="inlineStr"/>
     </row>
@@ -1423,30 +1481,32 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33544950041-2</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>100000</v>
+        <v>92000</v>
       </c>
       <c r="D34" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E34" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>TKRU 331264 5</t>
+          <t>NFLU 203537 0</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>2300</v>
+        <v>4500</v>
       </c>
       <c r="H34" t="n">
-        <v>20</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1454,25 +1514,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>100000</v>
+        <v>72000</v>
       </c>
       <c r="D35" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E35" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>NFLU 203458 5</t>
+          <t>LYSU 545712 9</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>23500</v>
+        <v>28386</v>
       </c>
       <c r="H35" t="n">
         <v>40</v>
@@ -1485,28 +1545,28 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>37804557797-0</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>100000</v>
+        <v>72000</v>
       </c>
       <c r="D36" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E36" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>ABEU 263315 6</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>27600</v>
       </c>
       <c r="H36" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I36" t="inlineStr"/>
     </row>
@@ -1516,28 +1576,28 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>100000</v>
+        <v>107600</v>
       </c>
       <c r="D37" t="n">
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>CLDU 961735 1</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>8518</v>
       </c>
       <c r="H37" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I37" t="inlineStr"/>
     </row>
@@ -1547,28 +1607,28 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>94000</v>
+        <v>107600</v>
       </c>
       <c r="D38" t="n">
         <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>CMAU 825245 1</t>
+          <t>MCMU 735118 9</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>17011</v>
+        <v>4800</v>
       </c>
       <c r="H38" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1578,28 +1638,28 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>94000</v>
+        <v>107600</v>
       </c>
       <c r="D39" t="n">
         <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TLLU 158811 1</t>
+          <t>TCKU 305135 8</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>26400</v>
+        <v>28620</v>
       </c>
       <c r="H39" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I39" t="inlineStr"/>
     </row>
@@ -1609,17 +1669,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>94000</v>
+        <v>107600</v>
       </c>
       <c r="D40" t="n">
         <v>90</v>
       </c>
       <c r="E40" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1640,17 +1700,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>33884961049-2</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>94000</v>
+        <v>107600</v>
       </c>
       <c r="D41" t="n">
         <v>90</v>
       </c>
       <c r="E41" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1664,6 +1724,690 @@
         <v>5</v>
       </c>
       <c r="I41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>33884961020-3</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>108000</v>
+      </c>
+      <c r="D42" t="n">
+        <v>90</v>
+      </c>
+      <c r="E42" t="n">
+        <v>18</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>CAIU 210709 4</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>28260</v>
+      </c>
+      <c r="H42" t="n">
+        <v>20</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>33884961020-3</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>108000</v>
+      </c>
+      <c r="D43" t="n">
+        <v>90</v>
+      </c>
+      <c r="E43" t="n">
+        <v>18</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>TWSU 971323 8</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>4800</v>
+      </c>
+      <c r="H43" t="n">
+        <v>20</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>33884961020-3</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>108000</v>
+      </c>
+      <c r="D44" t="n">
+        <v>90</v>
+      </c>
+      <c r="E44" t="n">
+        <v>18</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>DUMMY1</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" t="n">
+        <v>5</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>33884961020-3</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>108000</v>
+      </c>
+      <c r="D45" t="n">
+        <v>90</v>
+      </c>
+      <c r="E45" t="n">
+        <v>18</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>GCAU 795043 0</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>28120</v>
+      </c>
+      <c r="H45" t="n">
+        <v>20</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>33884961020-3</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>108000</v>
+      </c>
+      <c r="D46" t="n">
+        <v>90</v>
+      </c>
+      <c r="E46" t="n">
+        <v>18</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>DUMMY2</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>5</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>33884961020-3</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>108000</v>
+      </c>
+      <c r="D47" t="n">
+        <v>90</v>
+      </c>
+      <c r="E47" t="n">
+        <v>18</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>TCLU 226328 3</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>28160</v>
+      </c>
+      <c r="H47" t="n">
+        <v>20</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>31804557039-3</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>72000</v>
+      </c>
+      <c r="D48" t="n">
+        <v>60</v>
+      </c>
+      <c r="E48" t="n">
+        <v>21</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>TCLU 481269 6</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>4400</v>
+      </c>
+      <c r="H48" t="n">
+        <v>40</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>31804557039-3</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>72000</v>
+      </c>
+      <c r="D49" t="n">
+        <v>60</v>
+      </c>
+      <c r="E49" t="n">
+        <v>21</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>GMCU 238079 0</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>4800</v>
+      </c>
+      <c r="H49" t="n">
+        <v>20</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>37804557179-1</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D50" t="n">
+        <v>60</v>
+      </c>
+      <c r="E50" t="n">
+        <v>22</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>ABEU 252405 2</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>27960</v>
+      </c>
+      <c r="H50" t="n">
+        <v>20</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>37804557179-1</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D51" t="n">
+        <v>60</v>
+      </c>
+      <c r="E51" t="n">
+        <v>22</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>TKRU 331851 4</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>2300</v>
+      </c>
+      <c r="H51" t="n">
+        <v>20</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>37804557179-1</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>70000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>60</v>
+      </c>
+      <c r="E52" t="n">
+        <v>22</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>NWBU 010529 9</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>28020</v>
+      </c>
+      <c r="H52" t="n">
+        <v>20</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>33684953049-6</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>90</v>
+      </c>
+      <c r="E53" t="n">
+        <v>23</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>CAXU 696573 0</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>28320</v>
+      </c>
+      <c r="H53" t="n">
+        <v>20</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>33684953049-6</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D54" t="n">
+        <v>90</v>
+      </c>
+      <c r="E54" t="n">
+        <v>23</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>CLDU 962913 6</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>28836</v>
+      </c>
+      <c r="H54" t="n">
+        <v>40</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>33684953049-6</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D55" t="n">
+        <v>90</v>
+      </c>
+      <c r="E55" t="n">
+        <v>23</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>DUMMY1</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>5</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>33684953049-6</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D56" t="n">
+        <v>90</v>
+      </c>
+      <c r="E56" t="n">
+        <v>23</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>DUMMY2</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" t="n">
+        <v>5</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>33684953049-6</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D57" t="n">
+        <v>90</v>
+      </c>
+      <c r="E57" t="n">
+        <v>23</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>TCKU 133127 8</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>28380</v>
+      </c>
+      <c r="H57" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D58" t="n">
+        <v>90</v>
+      </c>
+      <c r="E58" t="n">
+        <v>24</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NWBU 103506 7</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>27800</v>
+      </c>
+      <c r="H58" t="n">
+        <v>20</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D59" t="n">
+        <v>90</v>
+      </c>
+      <c r="E59" t="n">
+        <v>24</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>TKRU 314169 2</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>2300</v>
+      </c>
+      <c r="H59" t="n">
+        <v>20</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D60" t="n">
+        <v>90</v>
+      </c>
+      <c r="E60" t="n">
+        <v>24</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>DUMMY1</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="n">
+        <v>5</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D61" t="n">
+        <v>90</v>
+      </c>
+      <c r="E61" t="n">
+        <v>24</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>TCKU 345040 3</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>25700</v>
+      </c>
+      <c r="H61" t="n">
+        <v>20</v>
+      </c>
+      <c r="I61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D62" t="n">
+        <v>90</v>
+      </c>
+      <c r="E62" t="n">
+        <v>24</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>DUMMY2</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>5</v>
+      </c>
+      <c r="I62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>37804952303-8</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>94000</v>
+      </c>
+      <c r="D63" t="n">
+        <v>90</v>
+      </c>
+      <c r="E63" t="n">
+        <v>24</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>ABEU 260711 5</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>25140</v>
+      </c>
+      <c r="H63" t="n">
+        <v>20</v>
+      </c>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Contents constraint works now
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,28 +481,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>37804556180-0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D2" t="n">
         <v>60</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NWBU 050535 6</t>
+          <t>TLLU 165639 2</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>28830</v>
+        <v>4400</v>
       </c>
       <c r="H2" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I2" t="inlineStr"/>
     </row>
@@ -512,30 +512,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>37804556180-0</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D3" t="n">
         <v>60</v>
       </c>
       <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>DHIU 114243 4</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>29000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>TKRU 303801 0</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>2300</v>
-      </c>
-      <c r="H3" t="n">
-        <v>20</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -543,7 +545,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37804556544-7</t>
+          <t>37804556674-2</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -553,22 +555,20 @@
         <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TANU 351116 0</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>31750</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>20</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -576,28 +576,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>37804556674-2</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -607,25 +607,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>37804556674-2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D6" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BTTU 223108 5</t>
+          <t>BIDU 497503 5</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>28180</v>
+        <v>32038</v>
       </c>
       <c r="H6" t="n">
         <v>20</v>
@@ -638,28 +638,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>37804556674-2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D7" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>CPWU 229894 0</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>7373</v>
       </c>
       <c r="H7" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -669,30 +669,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>108000</v>
+        <v>94000</v>
       </c>
       <c r="D8" t="n">
         <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>CMAU 825245 1</t>
+          <t>MCMU 635032 0</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>17011</v>
+        <v>30800</v>
       </c>
       <c r="H8" t="n">
-        <v>40</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -700,25 +702,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>33884962390-9</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>108000</v>
+        <v>94000</v>
       </c>
       <c r="D9" t="n">
         <v>90</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BTLU 269021 2</t>
+          <t>MCMU 735056 2</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>28090</v>
+        <v>4801</v>
       </c>
       <c r="H9" t="n">
         <v>20</v>
@@ -731,28 +733,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>72000</v>
+        <v>94000</v>
       </c>
       <c r="D10" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>CLDU 970465 1</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>8660</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I10" t="inlineStr"/>
     </row>
@@ -762,25 +764,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>31804557008-8</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>72000</v>
+        <v>94000</v>
       </c>
       <c r="D11" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PCVU 260064 7</t>
+          <t>PCVU 260136 6</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>29000</v>
+        <v>28000</v>
       </c>
       <c r="H11" t="n">
         <v>20</v>
@@ -793,28 +795,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>72000</v>
+        <v>94000</v>
       </c>
       <c r="D12" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E12" t="n">
         <v>6</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>HMCU 904434 0</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>23200</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -824,25 +826,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>31804557021-1</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>72000</v>
+        <v>94000</v>
       </c>
       <c r="D13" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E13" t="n">
         <v>6</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>PCVU 935014 9</t>
+          <t>RCLU 131060 3</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>31850</v>
+        <v>29840</v>
       </c>
       <c r="H13" t="n">
         <v>20</v>
@@ -855,28 +857,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>37804557351-6</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>107600</v>
+        <v>60000</v>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E14" t="n">
         <v>7</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>MCMU 635042 3</t>
+          <t>TLLU 158622 7</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>30040</v>
+        <v>4400</v>
       </c>
       <c r="H14" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -886,25 +888,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>37804557351-6</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>107600</v>
+        <v>60000</v>
       </c>
       <c r="D15" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E15" t="n">
         <v>7</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>TKRU 331264 5</t>
+          <t>PCVU 288038 4</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>2300</v>
+        <v>31000</v>
       </c>
       <c r="H15" t="n">
         <v>20</v>
@@ -917,28 +919,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>37804556642-9</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D16" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>GCAU 777634 0</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>30780</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I16" t="inlineStr"/>
     </row>
@@ -948,25 +950,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>37804556642-9</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D17" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>NWBU 082664 9</t>
+          <t>MEBU 331067 0</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>28880</v>
+        <v>4801</v>
       </c>
       <c r="H17" t="n">
         <v>20</v>
@@ -979,30 +981,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>37804556642-9</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>107600</v>
+        <v>70000</v>
       </c>
       <c r="D18" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>PAWU 310009 5</t>
         </is>
       </c>
       <c r="G18" t="n">
+        <v>32800</v>
+      </c>
+      <c r="H18" t="n">
+        <v>20</v>
+      </c>
+      <c r="I18" t="n">
         <v>1</v>
       </c>
-      <c r="H18" t="n">
-        <v>5</v>
-      </c>
-      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1010,28 +1014,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33884961594-7</t>
+          <t>31804557061-7</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>107600</v>
+        <v>72000</v>
       </c>
       <c r="D19" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>NWBU 103521 5</t>
+          <t>CMAU 909627 1</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>28800</v>
+        <v>11749</v>
       </c>
       <c r="H19" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I19" t="inlineStr"/>
     </row>
@@ -1041,28 +1045,28 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>31804557061-7</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D20" t="n">
         <v>60</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TCLU 483870 4</t>
+          <t>EXFU 878937 0</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>4400</v>
+        <v>30780</v>
       </c>
       <c r="H20" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I20" t="inlineStr"/>
     </row>
@@ -1072,7 +1076,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>33684556915-9</t>
+          <t>33684556902-7</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1082,18 +1086,18 @@
         <v>60</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ILBU 261007 6</t>
+          <t>TLLU 166110 4</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>28000</v>
+        <v>4400</v>
       </c>
       <c r="H21" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>
@@ -1103,7 +1107,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33684556902-7</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1113,20 +1117,22 @@
         <v>60</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ABEU 262887 0</t>
+          <t>DHIU 053205 8</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>32720</v>
+        <v>14000</v>
       </c>
       <c r="H22" t="n">
         <v>20</v>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1134,28 +1140,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D23" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>TKRU 313126 7</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>2300</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I23" t="inlineStr"/>
     </row>
@@ -1165,28 +1171,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33684556912-6</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>70000</v>
+        <v>107600</v>
       </c>
       <c r="D24" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>COUU 810204 9</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>32800</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1196,32 +1202,30 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D25" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E25" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>PCVU 288022 9</t>
+          <t>TWSU 971059 0</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>29280</v>
+        <v>28920</v>
       </c>
       <c r="H25" t="n">
         <v>20</v>
       </c>
-      <c r="I25" t="n">
-        <v>1</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1229,25 +1233,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D26" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E26" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TKRU 317044 8</t>
+          <t>TKCU 135014 4</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>2300</v>
+        <v>4801</v>
       </c>
       <c r="H26" t="n">
         <v>20</v>
@@ -1260,28 +1264,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>31804557042-7</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D27" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E27" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>DHDU 208805 2</t>
+          <t>GESU 695206 0</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>29500</v>
+        <v>13713</v>
       </c>
       <c r="H27" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1291,28 +1295,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>72000</v>
+        <v>107700</v>
       </c>
       <c r="D28" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E28" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>TLLU 158811 1</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>26400</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1322,28 +1326,28 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>31804557059-1</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>72000</v>
+        <v>107700</v>
       </c>
       <c r="D29" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E29" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ZTKU 735013 0</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>31770</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I29" t="inlineStr"/>
     </row>
@@ -1353,25 +1357,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>72000</v>
+        <v>107700</v>
       </c>
       <c r="D30" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E30" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PCVU 350020 0</t>
+          <t>BIDU 492892 2</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>27920</v>
+        <v>32000</v>
       </c>
       <c r="H30" t="n">
         <v>20</v>
@@ -1384,25 +1388,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>72000</v>
+        <v>107700</v>
       </c>
       <c r="D31" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E31" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TKRU 321509 6</t>
+          <t>MEBU 330049 7</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>2300</v>
+        <v>4801</v>
       </c>
       <c r="H31" t="n">
         <v>20</v>
@@ -1417,32 +1421,30 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>33684556890-4</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>72000</v>
+        <v>107700</v>
       </c>
       <c r="D32" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E32" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>MEBU 126421 4</t>
+          <t>GLDU 762731 2</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>28000</v>
+        <v>18202</v>
       </c>
       <c r="H32" t="n">
-        <v>20</v>
-      </c>
-      <c r="I32" t="n">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1450,28 +1452,28 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>92000</v>
+        <v>107600</v>
       </c>
       <c r="D33" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E33" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>CLDU 970371 6</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>7488</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I33" t="inlineStr"/>
     </row>
@@ -1481,32 +1483,30 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33544950041-2</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>92000</v>
+        <v>107600</v>
       </c>
       <c r="D34" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E34" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>NFLU 203537 0</t>
+          <t>CMAU 826520 6</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>4500</v>
+        <v>14064</v>
       </c>
       <c r="H34" t="n">
         <v>40</v>
       </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1514,28 +1514,28 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E35" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>LYSU 545712 9</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>28386</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I35" t="inlineStr"/>
     </row>
@@ -1545,30 +1545,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>37804557797-0</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>72000</v>
+        <v>107600</v>
       </c>
       <c r="D36" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>ABEU 263315 6</t>
+          <t>TLLU 158603 7</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>27600</v>
+        <v>4400</v>
       </c>
       <c r="H36" t="n">
-        <v>20</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1576,25 +1578,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D37" t="n">
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>CLDU 961735 1</t>
+          <t>SANU 751713 9</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>8518</v>
+        <v>7754</v>
       </c>
       <c r="H37" t="n">
         <v>40</v>
@@ -1607,28 +1609,28 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D38" t="n">
         <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>MCMU 735118 9</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1638,28 +1640,28 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D39" t="n">
         <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TCKU 305135 8</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>28620</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I39" t="inlineStr"/>
     </row>
@@ -1669,28 +1671,28 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D40" t="n">
         <v>90</v>
       </c>
       <c r="E40" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>CNEU 453016 9</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>7364</v>
       </c>
       <c r="H40" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I40" t="inlineStr"/>
     </row>
@@ -1700,25 +1702,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>33884961049-2</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D41" t="n">
         <v>90</v>
       </c>
       <c r="E41" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
         <v>5</v>
@@ -1731,28 +1733,28 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>108000</v>
+        <v>107700</v>
       </c>
       <c r="D42" t="n">
         <v>90</v>
       </c>
       <c r="E42" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>CAIU 210709 4</t>
+          <t>SEGU 573325 2</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>28260</v>
+        <v>24731</v>
       </c>
       <c r="H42" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I42" t="inlineStr"/>
     </row>
@@ -1762,28 +1764,28 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>108000</v>
+        <v>107700</v>
       </c>
       <c r="D43" t="n">
         <v>90</v>
       </c>
       <c r="E43" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>TWSU 971323 8</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>4800</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I43" t="inlineStr"/>
     </row>
@@ -1793,30 +1795,32 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>108000</v>
+        <v>107700</v>
       </c>
       <c r="D44" t="n">
         <v>90</v>
       </c>
       <c r="E44" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>SANU 799934 4</t>
         </is>
       </c>
       <c r="G44" t="n">
+        <v>8752</v>
+      </c>
+      <c r="H44" t="n">
+        <v>40</v>
+      </c>
+      <c r="I44" t="n">
         <v>1</v>
       </c>
-      <c r="H44" t="n">
-        <v>5</v>
-      </c>
-      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1824,25 +1828,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557045-0</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D45" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E45" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>GCAU 795043 0</t>
+          <t>MEDU 220821 2</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>28120</v>
+        <v>26408</v>
       </c>
       <c r="H45" t="n">
         <v>20</v>
@@ -1855,28 +1859,28 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557045-0</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E46" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>MCMU 735068 6</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>4801</v>
       </c>
       <c r="H46" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I46" t="inlineStr"/>
     </row>
@@ -1886,25 +1890,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>33884961020-3</t>
+          <t>31804557045-0</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D47" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E47" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>TCLU 226328 3</t>
+          <t>PAWU 310006 9</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>28160</v>
+        <v>32800</v>
       </c>
       <c r="H47" t="n">
         <v>20</v>
@@ -1917,28 +1921,28 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D48" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E48" t="n">
         <v>21</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>TCLU 481269 6</t>
+          <t>BGBU 080494 3</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>4400</v>
+        <v>29000</v>
       </c>
       <c r="H48" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I48" t="inlineStr"/>
     </row>
@@ -1948,25 +1952,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>31804557039-3</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>72000</v>
+        <v>108000</v>
       </c>
       <c r="D49" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E49" t="n">
         <v>21</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>GMCU 238079 0</t>
+          <t>HILU 331015 7</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>4800</v>
+        <v>4801</v>
       </c>
       <c r="H49" t="n">
         <v>20</v>
@@ -1979,28 +1983,28 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D50" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E50" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>ABEU 252405 2</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>27960</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I50" t="inlineStr"/>
     </row>
@@ -2010,25 +2014,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D51" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E51" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>TKRU 331851 4</t>
+          <t>TCVU 361832 5</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>2300</v>
+        <v>27460</v>
       </c>
       <c r="H51" t="n">
         <v>20</v>
@@ -2041,28 +2045,28 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>37804557179-1</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D52" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E52" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>NWBU 010529 9</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>28020</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I52" t="inlineStr"/>
     </row>
@@ -2072,30 +2076,32 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>100000</v>
+        <v>108000</v>
       </c>
       <c r="D53" t="n">
         <v>90</v>
       </c>
       <c r="E53" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>CAXU 696573 0</t>
+          <t>BTTU 224149 0</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>28320</v>
+        <v>27860</v>
       </c>
       <c r="H53" t="n">
         <v>20</v>
       </c>
-      <c r="I53" t="inlineStr"/>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2103,25 +2109,25 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33684556908-4</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>100000</v>
+        <v>70000</v>
       </c>
       <c r="D54" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E54" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>CLDU 962913 6</t>
+          <t>CSFU 967769 0</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>28836</v>
+        <v>16755</v>
       </c>
       <c r="H54" t="n">
         <v>40</v>
@@ -2134,28 +2140,28 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>33684556908-4</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>100000</v>
+        <v>70000</v>
       </c>
       <c r="D55" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E55" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>DUMMY1</t>
+          <t>PAWU 310008 0</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>32600</v>
       </c>
       <c r="H55" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I55" t="inlineStr"/>
     </row>
@@ -2165,28 +2171,28 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>31804557843-8</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>100000</v>
+        <v>70000</v>
       </c>
       <c r="D56" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E56" t="n">
         <v>23</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>DUMMY2</t>
+          <t>TLLU 158601 6</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>4400</v>
       </c>
       <c r="H56" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I56" t="inlineStr"/>
     </row>
@@ -2196,25 +2202,25 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>33684953049-6</t>
+          <t>31804557843-8</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>100000</v>
+        <v>70000</v>
       </c>
       <c r="D57" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E57" t="n">
         <v>23</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>TCKU 133127 8</t>
+          <t>GCAU 793007 5</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>28380</v>
+        <v>30800</v>
       </c>
       <c r="H57" t="n">
         <v>20</v>
@@ -2227,30 +2233,32 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>37804557177-5</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D58" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E58" t="n">
         <v>24</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>NWBU 103506 7</t>
+          <t>TLLU 164938 8</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>27800</v>
+        <v>4400</v>
       </c>
       <c r="H58" t="n">
-        <v>20</v>
-      </c>
-      <c r="I58" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2258,156 +2266,30 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>37804952303-8</t>
+          <t>37804557177-5</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D59" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E59" t="n">
         <v>24</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>TKRU 314169 2</t>
+          <t>MCMU 735087 6</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>2300</v>
+        <v>4801</v>
       </c>
       <c r="H59" t="n">
         <v>20</v>
       </c>
       <c r="I59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C60" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D60" t="n">
-        <v>90</v>
-      </c>
-      <c r="E60" t="n">
-        <v>24</v>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>DUMMY1</t>
-        </is>
-      </c>
-      <c r="G60" t="n">
-        <v>1</v>
-      </c>
-      <c r="H60" t="n">
-        <v>5</v>
-      </c>
-      <c r="I60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C61" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D61" t="n">
-        <v>90</v>
-      </c>
-      <c r="E61" t="n">
-        <v>24</v>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>TCKU 345040 3</t>
-        </is>
-      </c>
-      <c r="G61" t="n">
-        <v>25700</v>
-      </c>
-      <c r="H61" t="n">
-        <v>20</v>
-      </c>
-      <c r="I61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C62" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D62" t="n">
-        <v>90</v>
-      </c>
-      <c r="E62" t="n">
-        <v>24</v>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>DUMMY2</t>
-        </is>
-      </c>
-      <c r="G62" t="n">
-        <v>1</v>
-      </c>
-      <c r="H62" t="n">
-        <v>5</v>
-      </c>
-      <c r="I62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>37804952303-8</t>
-        </is>
-      </c>
-      <c r="C63" t="n">
-        <v>94000</v>
-      </c>
-      <c r="D63" t="n">
-        <v>90</v>
-      </c>
-      <c r="E63" t="n">
-        <v>24</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>ABEU 260711 5</t>
-        </is>
-      </c>
-      <c r="G63" t="n">
-        <v>25140</v>
-      </c>
-      <c r="H63" t="n">
-        <v>20</v>
-      </c>
-      <c r="I63" t="n">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Removed a lot of printing, some code cleanup
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -481,28 +481,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>37804557177-5</t>
+          <t>37804556180-0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D2" t="n">
         <v>60</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>MCMU 735068 6</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>4801</v>
       </c>
       <c r="H2" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I2" t="inlineStr"/>
     </row>
@@ -512,25 +512,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>37804557177-5</t>
+          <t>37804556180-0</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D3" t="n">
         <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CMAU 909627 1</t>
+          <t>GESU 695206 0</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>11749</v>
+        <v>13713</v>
       </c>
       <c r="H3" t="n">
         <v>40</v>
@@ -543,7 +543,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37804557177-5</t>
+          <t>37804556674-2</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -553,18 +553,18 @@
         <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Empty Space 2</t>
+          <t>TLLU 165639 2</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>4400</v>
       </c>
       <c r="H4" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I4" t="inlineStr"/>
     </row>
@@ -574,7 +574,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>31804557843-8</t>
+          <t>37804556674-2</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -584,18 +584,18 @@
         <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TLLU 158622 7</t>
+          <t>BGBU 080494 3</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4400</v>
+        <v>29000</v>
       </c>
       <c r="H5" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I5" t="inlineStr"/>
     </row>
@@ -605,28 +605,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31804557843-8</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D6" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>MCMU 735056 2</t>
+          <t>SANU 799934 4</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4801</v>
+        <v>8752</v>
       </c>
       <c r="H6" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I6" t="inlineStr"/>
     </row>
@@ -636,28 +636,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>33684556908-4</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D7" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>TWSU 971059 0</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>28920</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -667,28 +667,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33684556908-4</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>MEBU 331067 0</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>4801</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I8" t="inlineStr"/>
     </row>
@@ -698,28 +698,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>33684556908-4</t>
+          <t>37804953046-2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>70000</v>
+        <v>94000</v>
       </c>
       <c r="D9" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BGBU 080494 3</t>
+          <t>CMAU 909627 1</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>29000</v>
+        <v>11749</v>
       </c>
       <c r="H9" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -729,30 +729,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804557351-6</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>108000</v>
+        <v>60000</v>
       </c>
       <c r="D10" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>SANU 751713 9</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>7754</v>
       </c>
       <c r="H10" t="n">
-        <v>5</v>
-      </c>
-      <c r="I10" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -760,25 +762,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804557351-6</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>108000</v>
+        <v>60000</v>
       </c>
       <c r="D11" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>BIDU 492892 2</t>
+          <t>TKCU 135014 4</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>32000</v>
+        <v>4801</v>
       </c>
       <c r="H11" t="n">
         <v>20</v>
@@ -791,28 +793,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804556642-9</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D12" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Empty Space 2</t>
+          <t>CNEU 453016 9</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>7364</v>
       </c>
       <c r="H12" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I12" t="inlineStr"/>
     </row>
@@ -822,28 +824,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>37804556642-9</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>108000</v>
+        <v>70000</v>
       </c>
       <c r="D13" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>GLDU 762731 2</t>
+          <t>PAWU 310006 9</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>18202</v>
+        <v>32800</v>
       </c>
       <c r="H13" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I13" t="inlineStr"/>
     </row>
@@ -853,28 +855,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>33884961383-5</t>
+          <t>31804557061-7</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>108000</v>
+        <v>72000</v>
       </c>
       <c r="D14" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>PCVU 288038 4</t>
+          <t>TLLU 158622 7</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>31000</v>
+        <v>4400</v>
       </c>
       <c r="H14" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I14" t="inlineStr"/>
     </row>
@@ -884,7 +886,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>31804557045-0</t>
+          <t>31804557061-7</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -894,18 +896,18 @@
         <v>60</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>CMAU 826520 6</t>
+          <t>DHIU 114243 4</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>14064</v>
+        <v>29000</v>
       </c>
       <c r="H15" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I15" t="inlineStr"/>
     </row>
@@ -915,32 +917,30 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>31804557045-0</t>
+          <t>33684556902-7</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D16" t="n">
         <v>60</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>PAWU 310009 5</t>
+          <t>BIDU 497503 5</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>32800</v>
+        <v>32038</v>
       </c>
       <c r="H16" t="n">
         <v>20</v>
       </c>
-      <c r="I16" t="n">
-        <v>1</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -948,28 +948,28 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33684556902-7</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>107700</v>
+        <v>70000</v>
       </c>
       <c r="D17" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>MCMU 735056 2</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>4801</v>
       </c>
       <c r="H17" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I17" t="inlineStr"/>
     </row>
@@ -979,25 +979,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33684556902-7</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>107700</v>
+        <v>70000</v>
       </c>
       <c r="D18" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>PCVU 260136 6</t>
+          <t>PAWU 310008 0</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>28000</v>
+        <v>32600</v>
       </c>
       <c r="H18" t="n">
         <v>20</v>
@@ -1010,25 +1010,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D19" t="n">
         <v>90</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SANU 751713 9</t>
+          <t>TLLU 166110 4</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>7754</v>
+        <v>4400</v>
       </c>
       <c r="H19" t="n">
         <v>40</v>
@@ -1041,28 +1041,28 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D20" t="n">
         <v>90</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>PAWU 310006 9</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>32800</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I20" t="inlineStr"/>
     </row>
@@ -1072,17 +1072,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>33884961423-9</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D21" t="n">
         <v>90</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1103,25 +1103,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>33884962416-2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D22" t="n">
         <v>90</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>CNEU 453016 9</t>
+          <t>TLLU 158603 7</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>7364</v>
+        <v>4400</v>
       </c>
       <c r="H22" t="n">
         <v>40</v>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1144,18 +1144,18 @@
         <v>90</v>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>TLLU 158601 6</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>4400</v>
       </c>
       <c r="H23" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I23" t="inlineStr"/>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1175,11 +1175,11 @@
         <v>90</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Empty Space 2</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>33884961176-3</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1206,18 +1206,18 @@
         <v>90</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>GESU 695206 0</t>
+          <t>BTTU 224149 0</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>13713</v>
+        <v>27860</v>
       </c>
       <c r="H25" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I25" t="inlineStr"/>
     </row>
@@ -1227,28 +1227,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>33884962434-5</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D26" t="n">
         <v>90</v>
       </c>
       <c r="E26" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TLLU 165639 2</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>4400</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I26" t="inlineStr"/>
     </row>
@@ -1258,28 +1258,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>33884962434-5</t>
+          <t>33884961166-4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D27" t="n">
         <v>90</v>
       </c>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>MEDU 220821 2</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>26408</v>
       </c>
       <c r="H27" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1299,18 +1299,18 @@
         <v>90</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Empty Space 2</t>
+          <t>CMAU 826520 6</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>14064</v>
       </c>
       <c r="H28" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="I28" t="inlineStr"/>
     </row>
@@ -1330,18 +1330,18 @@
         <v>90</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>TLLU 166110 4</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>4400</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I29" t="inlineStr"/>
     </row>
@@ -1351,30 +1351,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D30" t="n">
         <v>90</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>MCMU 735087 6</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>4801</v>
       </c>
       <c r="H30" t="n">
-        <v>5</v>
-      </c>
-      <c r="I30" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1382,25 +1384,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D31" t="n">
         <v>90</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>BIDU 497503 5</t>
+          <t>RCLU 131060 3</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>32038</v>
+        <v>29840</v>
       </c>
       <c r="H31" t="n">
         <v>20</v>
@@ -1413,28 +1415,28 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33884962434-5</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>107700</v>
+        <v>107600</v>
       </c>
       <c r="D32" t="n">
         <v>90</v>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>CSFU 967769 0</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>16755</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="I32" t="inlineStr"/>
     </row>
@@ -1444,7 +1446,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1454,18 +1456,18 @@
         <v>90</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Empty Space 2</t>
+          <t>PCVU 288038 4</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>31000</v>
       </c>
       <c r="H33" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I33" t="inlineStr"/>
     </row>
@@ -1475,7 +1477,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>33884961166-4</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1485,15 +1487,15 @@
         <v>90</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>PAWU 310008 0</t>
+          <t>MEBU 331067 0</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>32600</v>
+        <v>4801</v>
       </c>
       <c r="H34" t="n">
         <v>20</v>
@@ -1506,32 +1508,30 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D35" t="n">
         <v>90</v>
       </c>
       <c r="E35" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>TLLU 164938 8</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4400</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>40</v>
-      </c>
-      <c r="I35" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1539,28 +1539,28 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D36" t="n">
         <v>90</v>
       </c>
       <c r="E36" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>GCAU 777634 0</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>30780</v>
       </c>
       <c r="H36" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I36" t="inlineStr"/>
     </row>
@@ -1570,17 +1570,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D37" t="n">
         <v>90</v>
       </c>
       <c r="E37" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1601,28 +1601,28 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>33884962416-2</t>
+          <t>33884961176-3</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>107600</v>
+        <v>107700</v>
       </c>
       <c r="D38" t="n">
         <v>90</v>
       </c>
       <c r="E38" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>TLLU 158601 6</t>
+          <t>EXFU 878937 0</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>4400</v>
+        <v>30780</v>
       </c>
       <c r="H38" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I38" t="inlineStr"/>
     </row>
@@ -1632,28 +1632,28 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>33684556902-7</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>70000</v>
+        <v>107700</v>
       </c>
       <c r="D39" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E39" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TKCU 135014 4</t>
+          <t>GLDU 762731 2</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>4801</v>
+        <v>18202</v>
       </c>
       <c r="H39" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I39" t="inlineStr"/>
     </row>
@@ -1663,28 +1663,28 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>33684556902-7</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>70000</v>
+        <v>107700</v>
       </c>
       <c r="D40" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E40" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>RCLU 131060 3</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>29840</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I40" t="inlineStr"/>
     </row>
@@ -1694,28 +1694,28 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>33684556902-7</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>70000</v>
+        <v>107700</v>
       </c>
       <c r="D41" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E41" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>MCMU 735068 6</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>4801</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I41" t="inlineStr"/>
     </row>
@@ -1725,30 +1725,32 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>31804557061-7</t>
+          <t>33884961423-9</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>72000</v>
+        <v>107700</v>
       </c>
       <c r="D42" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E42" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>SEGU 573325 2</t>
+          <t>CSFU 967769 0</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>24731</v>
+        <v>16755</v>
       </c>
       <c r="H42" t="n">
         <v>40</v>
       </c>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1756,7 +1758,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>31804557061-7</t>
+          <t>31804557045-0</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1766,22 +1768,20 @@
         <v>60</v>
       </c>
       <c r="E43" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>BTTU 224149 0</t>
+          <t>GCAU 793007 5</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>27860</v>
+        <v>30800</v>
       </c>
       <c r="H43" t="n">
         <v>20</v>
       </c>
-      <c r="I43" t="n">
-        <v>1</v>
-      </c>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1789,25 +1789,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>37804556642-9</t>
+          <t>31804557045-0</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D44" t="n">
         <v>60</v>
       </c>
       <c r="E44" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>GCAU 777634 0</t>
+          <t>CPWU 229894 0</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>30780</v>
+        <v>7373</v>
       </c>
       <c r="H44" t="n">
         <v>20</v>
@@ -1820,30 +1820,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>37804556642-9</t>
+          <t>31804557045-0</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>70000</v>
+        <v>72000</v>
       </c>
       <c r="D45" t="n">
         <v>60</v>
       </c>
       <c r="E45" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>MCMU 735087 6</t>
+          <t>MCMU 635032 0</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>4801</v>
+        <v>30800</v>
       </c>
       <c r="H45" t="n">
         <v>20</v>
       </c>
-      <c r="I45" t="inlineStr"/>
+      <c r="I45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1851,28 +1853,28 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>37804556642-9</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="D46" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E46" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>EXFU 878937 0</t>
+          <t>SEGU 573325 2</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>30780</v>
+        <v>24731</v>
       </c>
       <c r="H46" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I46" t="inlineStr"/>
     </row>
@@ -1882,32 +1884,30 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>37804557351-6</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>60000</v>
+        <v>108000</v>
       </c>
       <c r="D47" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E47" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>TLLU 158603 7</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>4400</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>40</v>
-      </c>
-      <c r="I47" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1915,25 +1915,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>37804557351-6</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>60000</v>
+        <v>108000</v>
       </c>
       <c r="D48" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E48" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>GCAU 793007 5</t>
+          <t>DHIU 053205 8</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>30800</v>
+        <v>14000</v>
       </c>
       <c r="H48" t="n">
         <v>20</v>
@@ -1946,30 +1946,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>94000</v>
+        <v>108000</v>
       </c>
       <c r="D49" t="n">
         <v>90</v>
       </c>
       <c r="E49" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Empty Space 1</t>
+          <t>TWSU 971059 0</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>28920</v>
       </c>
       <c r="H49" t="n">
-        <v>5</v>
-      </c>
-      <c r="I49" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1977,28 +1979,28 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33884961383-5</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>94000</v>
+        <v>108000</v>
       </c>
       <c r="D50" t="n">
         <v>90</v>
       </c>
       <c r="E50" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>TCVU 361832 5</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>27460</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I50" t="inlineStr"/>
     </row>
@@ -2008,28 +2010,28 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33684556908-4</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D51" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E51" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Empty Space 2</t>
+          <t>Empty Space 1</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I51" t="inlineStr"/>
     </row>
@@ -2039,32 +2041,30 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33684556908-4</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D52" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E52" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>DHIU 053205 8</t>
+          <t>TCVU 361832 5</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>14000</v>
+        <v>27460</v>
       </c>
       <c r="H52" t="n">
         <v>20</v>
       </c>
-      <c r="I52" t="n">
-        <v>1</v>
-      </c>
+      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2072,25 +2072,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33684556908-4</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D53" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E53" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>HILU 331015 7</t>
+          <t>PAWU 310009 5</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>4801</v>
+        <v>32800</v>
       </c>
       <c r="H53" t="n">
         <v>20</v>
@@ -2103,28 +2103,28 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>37804953046-2</t>
+          <t>33684556908-4</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>94000</v>
+        <v>70000</v>
       </c>
       <c r="D54" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E54" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>MEDU 220821 2</t>
+          <t>Empty Space 2</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>26408</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I54" t="inlineStr"/>
     </row>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>37804556674-2</t>
+          <t>31804557843-8</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -2144,15 +2144,15 @@
         <v>60</v>
       </c>
       <c r="E55" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>SANU 799934 4</t>
+          <t>TLLU 164938 8</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>8752</v>
+        <v>4400</v>
       </c>
       <c r="H55" t="n">
         <v>40</v>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>37804556674-2</t>
+          <t>31804557843-8</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -2177,7 +2177,7 @@
         <v>60</v>
       </c>
       <c r="E56" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2190,9 +2190,7 @@
       <c r="H56" t="n">
         <v>20</v>
       </c>
-      <c r="I56" t="n">
-        <v>1</v>
-      </c>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2200,32 +2198,30 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>37804556180-0</t>
+          <t>37804557177-5</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D57" t="n">
         <v>60</v>
       </c>
       <c r="E57" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>DHIU 114243 4</t>
+          <t>PCVU 260136 6</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>29000</v>
+        <v>28000</v>
       </c>
       <c r="H57" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="n">
-        <v>1</v>
-      </c>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2233,25 +2229,25 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>37804556180-0</t>
+          <t>37804557177-5</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D58" t="n">
         <v>60</v>
       </c>
       <c r="E58" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>CPWU 229894 0</t>
+          <t>HILU 331015 7</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>7373</v>
+        <v>4801</v>
       </c>
       <c r="H58" t="n">
         <v>20</v>
@@ -2264,32 +2260,30 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>37804556180-0</t>
+          <t>37804557177-5</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>72000</v>
+        <v>70000</v>
       </c>
       <c r="D59" t="n">
         <v>60</v>
       </c>
       <c r="E59" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>MCMU 635032 0</t>
+          <t>BIDU 492892 2</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>30800</v>
+        <v>32000</v>
       </c>
       <c r="H59" t="n">
         <v>20</v>
       </c>
-      <c r="I59" t="n">
-        <v>1</v>
-      </c>
+      <c r="I59" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>